<commit_message>
Correct voc4cat-prefix in Excel template
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\nfdi4cat\gh-dalito\voc4cat-template\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D4E7DC-20C2-4CA2-B23B-F550D63A5BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5279714C-CB90-44D9-8E9A-A63F98EB4A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>https://example.org/new/</t>
   </si>
   <si>
-    <t>https://w3id.org/nfdi4cat/voc4cat/</t>
-  </si>
-  <si>
     <t>The spreadsheet is processed with voc4cat which extends vocexcel for the voc4cat-based repositories.</t>
   </si>
   <si>
@@ -1243,9 +1240,6 @@
   </si>
   <si>
     <t>revision</t>
-  </si>
-  <si>
-    <t>2023-03a</t>
   </si>
   <si>
     <r>
@@ -1574,6 +1568,12 @@
   </si>
   <si>
     <t>Concepts*</t>
+  </si>
+  <si>
+    <t>https://w3id.org/nfdi4cat/voc4cat_</t>
+  </si>
+  <si>
+    <t>2023-06a</t>
   </si>
 </sst>
 </file>
@@ -1914,66 +1914,6 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFD9EAD3"/>
       </font>
@@ -2038,6 +1978,66 @@
           <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2110,25 +2110,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I20" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I20" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A2:I20" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9FE8BFF8-A78B-448D-A131-9A0D98C9F3D7}" name="Concept IRI*" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{86239A34-9941-49E0-9977-1A07DF28C21F}" name="Preferred Label*" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3DDC515C-66BD-4D72-9F90-11ECCC367C9E}" name="Pref. Label Language Code" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{DFD56705-3476-4395-8E82-4BA1B2D9FB6C}" name="Definition*" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{73464C4B-4966-4F01-A700-A547FE1A016C}" name="Def. Language Code" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{A1F0E882-A632-4EAB-9875-D263174AB2AC}" name="Alternate Labels" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{45F1B146-1861-40A5-A017-E62DF2AF1EDE}" name="Children IRIs" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{6CD00781-D481-43C6-9E4B-C9105CE6954A}" name="Provenance*" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{C6B9560F-7DE1-43A3-AE9F-6EEE88487995}" name="Source Vocab URI" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9FE8BFF8-A78B-448D-A131-9A0D98C9F3D7}" name="Concept IRI*" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{86239A34-9941-49E0-9977-1A07DF28C21F}" name="Preferred Label*" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{3DDC515C-66BD-4D72-9F90-11ECCC367C9E}" name="Pref. Label Language Code" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{DFD56705-3476-4395-8E82-4BA1B2D9FB6C}" name="Definition*" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{73464C4B-4966-4F01-A700-A547FE1A016C}" name="Def. Language Code" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A1F0E882-A632-4EAB-9875-D263174AB2AC}" name="Alternate Labels" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{45F1B146-1861-40A5-A017-E62DF2AF1EDE}" name="Children IRIs" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{6CD00781-D481-43C6-9E4B-C9105CE6954A}" name="Provenance*" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{C6B9560F-7DE1-43A3-AE9F-6EEE88487995}" name="Source Vocab URI" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F0019B54-5478-4B2D-B2DC-B81783F2E087}" name="concept_relations" displayName="concept_relations" ref="A2:F20" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F0019B54-5478-4B2D-B2DC-B81783F2E087}" name="concept_relations" displayName="concept_relations" ref="A2:F20" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A2:F20" xr:uid="{F0019B54-5478-4B2D-B2DC-B81783F2E087}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{94539CED-3865-4A8C-AC09-EF3C512E3567}" name="Concept IRI*"/>
@@ -2143,21 +2143,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6ED60B90-A5EC-4F1E-9CF2-D984C20452D6}" name="collections" displayName="collections" ref="A2:E20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6ED60B90-A5EC-4F1E-9CF2-D984C20452D6}" name="collections" displayName="collections" ref="A2:E20" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:E20" xr:uid="{6ED60B90-A5EC-4F1E-9CF2-D984C20452D6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{93EAAE4B-8D60-4F74-8745-A2195B7A0D5C}" name="Collection IRI" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{134406ED-31FC-425A-82E8-23EE8F1B82A5}" name="Preferred Label" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CA3ED009-9BFA-4919-9F93-47D10664A305}" name="Definition" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E52278B9-419C-4E49-BF0A-3898B2077694}" name="Member IRIs" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E12774E7-E938-4E4B-A0FF-F29983D1E4C6}" name="Provenance" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{93EAAE4B-8D60-4F74-8745-A2195B7A0D5C}" name="Collection IRI" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{134406ED-31FC-425A-82E8-23EE8F1B82A5}" name="Preferred Label" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{CA3ED009-9BFA-4919-9F93-47D10664A305}" name="Definition" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E52278B9-419C-4E49-BF0A-3898B2077694}" name="Member IRIs" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E12774E7-E938-4E4B-A0FF-F29983D1E4C6}" name="Provenance" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B20" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B20" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:B20" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A30D4DF8-3B4A-4F43-9882-EDFDD8090F9E}" name="Prefix"/>
@@ -2469,7 +2469,9 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2486,7 +2488,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2495,15 +2497,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2564,12 +2566,12 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>32</v>
@@ -2577,7 +2579,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>34</v>
@@ -2585,10 +2587,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2596,29 +2598,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2658,7 +2660,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2726,7 +2728,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2739,10 +2741,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2752,10 +2754,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2776,7 +2778,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3151,7 +3153,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3605,7 +3607,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3905,7 +3907,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -4062,7 +4064,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4186,7 +4188,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4243,18 +4245,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E148" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="E148" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5289,32 +5291,32 @@
     <mergeCell ref="B116:J129"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B4 B46:B86">
-    <cfRule type="containsBlanks" dxfId="25" priority="7">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B44">
-    <cfRule type="containsBlanks" dxfId="24" priority="6">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="containsBlanks" dxfId="23" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(B88))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B116">
-    <cfRule type="containsBlanks" dxfId="22" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(B116))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B131">
-    <cfRule type="containsBlanks" dxfId="21" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(B131))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143:B147">
-    <cfRule type="containsBlanks" dxfId="20" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B143))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5350,7 +5352,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5358,10 +5360,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>30</v>
@@ -5372,10 +5374,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5386,10 +5388,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5403,10 +5405,10 @@
         <v>44995</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5417,10 +5419,10 @@
         <v>44995</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5431,10 +5433,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5445,10 +5447,10 @@
         <v>29</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -5456,10 +5458,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>108</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>109</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -5470,7 +5472,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>12</v>
@@ -5484,7 +5486,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -6519,7 +6521,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6530,19 +6532,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -6553,78 +6555,78 @@
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="D3" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I5" s="9"/>
     </row>
@@ -6825,7 +6827,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6833,27 +6835,27 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
@@ -7383,7 +7385,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -7391,19 +7393,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7579,7 +7581,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -7591,7 +7593,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat/" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add checking based on config to gh-action (#25)
* Add checking based on config to gh-action

- artifact now have the date as part of their name (and run id)
- example vocabulary updated to match idranges.toml

* Update documentation in READMEs
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5279714C-CB90-44D9-8E9A-A63F98EB4A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C880E2E-DB15-4A6E-A8DA-92366AAD00A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="116">
   <si>
     <t>0.4.3</t>
   </si>
@@ -198,18 +198,9 @@
     <t>https://github.com/nfdi4cat/vocexcel</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>voc4cat</t>
-  </si>
-  <si>
     <t>https://example.org/</t>
   </si>
   <si>
-    <t>https://example.org/new/</t>
-  </si>
-  <si>
     <t>The spreadsheet is processed with voc4cat which extends vocexcel for the voc4cat-based repositories.</t>
   </si>
   <si>
@@ -282,18 +273,12 @@
     <t>Concept Scheme*</t>
   </si>
   <si>
-    <t>ex:test_</t>
-  </si>
-  <si>
     <t>Test-of-Voc4Cat</t>
   </si>
   <si>
     <t>A test vocabulary for the voc4cat template</t>
   </si>
   <si>
-    <t>ex:c01</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -301,9 +286,6 @@
   </si>
   <si>
     <t>https://www.w3.org/TR/2010/NOTE-curie-20101216/</t>
-  </si>
-  <si>
-    <t>ex:c02</t>
   </si>
   <si>
     <t>URI</t>
@@ -343,19 +325,7 @@
     <t>IRI</t>
   </si>
   <si>
-    <t>ex:c03</t>
-  </si>
-  <si>
-    <t>ex:col1</t>
-  </si>
-  <si>
     <t>Linked data term</t>
-  </si>
-  <si>
-    <t>ex:c01, ex:c02, ex:c03</t>
-  </si>
-  <si>
-    <t>voc4cat-template</t>
   </si>
   <si>
     <t>Collection of term related to linked data.</t>
@@ -439,9 +409,6 @@
   </si>
   <si>
     <t>If you need help, feel free to create issues on github for your questions.</t>
-  </si>
-  <si>
-    <t>v2023-03-10</t>
   </si>
   <si>
     <t>Version specifier for the vocabulary</t>
@@ -1570,10 +1537,34 @@
     <t>Concepts*</t>
   </si>
   <si>
-    <t>https://w3id.org/nfdi4cat/voc4cat_</t>
-  </si>
-  <si>
     <t>2023-06a</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-2345-6789 Sofia Garcia</t>
+  </si>
+  <si>
+    <t>v2023-07-25</t>
+  </si>
+  <si>
+    <t>exvoc</t>
+  </si>
+  <si>
+    <t>https://example.org/exvoc</t>
+  </si>
+  <si>
+    <t>exvoc:0000001</t>
+  </si>
+  <si>
+    <t>exvoc:0000002</t>
+  </si>
+  <si>
+    <t>exvoc:0000003</t>
+  </si>
+  <si>
+    <t>exvoc:0000010</t>
+  </si>
+  <si>
+    <t>exvoc:0000001, exvoc:0000002, exvoc:0000003</t>
   </si>
 </sst>
 </file>
@@ -2469,8 +2460,8 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,7 +2479,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2497,15 +2488,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2566,12 +2557,12 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>32</v>
@@ -2579,7 +2570,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>34</v>
@@ -2587,10 +2578,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2598,29 +2589,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2660,7 +2651,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2728,7 +2719,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2741,10 +2732,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2754,10 +2745,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2778,7 +2769,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3153,7 +3144,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3607,7 +3598,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3907,7 +3898,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -4064,7 +4055,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4188,7 +4179,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4245,18 +4236,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5338,8 +5329,8 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5352,7 +5343,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5360,10 +5351,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>30</v>
@@ -5374,10 +5365,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5388,10 +5379,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5405,10 +5396,10 @@
         <v>44995</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5416,13 +5407,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="16">
-        <v>44995</v>
+        <v>45132</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5433,10 +5424,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5447,10 +5438,10 @@
         <v>29</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -5458,10 +5449,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -5472,7 +5463,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>12</v>
@@ -5486,7 +5477,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -6503,7 +6494,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6521,7 +6512,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6532,19 +6523,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -6555,80 +6546,86 @@
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="9"/>
+      <c r="H4" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="9"/>
+      <c r="H5" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
@@ -6638,7 +6635,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6797,7 +6794,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -6816,7 +6813,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6827,7 +6824,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6835,27 +6832,27 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
@@ -7357,7 +7354,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7385,27 +7382,27 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>87</v>
+        <v>115</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7541,10 +7538,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7565,23 +7562,15 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -7592,12 +7581,11 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat/" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://example.org/new/" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix typos in template
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C880E2E-DB15-4A6E-A8DA-92366AAD00A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333FB821-20CB-452C-9828-FF39C2B47E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
   <si>
     <t>0.4.3</t>
   </si>
@@ -183,9 +183,6 @@
     <t>NFDI4Cat</t>
   </si>
   <si>
-    <t>Required: URI or CURI</t>
-  </si>
-  <si>
     <t>Collection IRI</t>
   </si>
   <si>
@@ -198,9 +195,18 @@
     <t>https://github.com/nfdi4cat/vocexcel</t>
   </si>
   <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>voc4cat</t>
+  </si>
+  <si>
     <t>https://example.org/</t>
   </si>
   <si>
+    <t>https://example.org/new/</t>
+  </si>
+  <si>
     <t>The spreadsheet is processed with voc4cat which extends vocexcel for the voc4cat-based repositories.</t>
   </si>
   <si>
@@ -255,9 +261,6 @@
     <t>Date of creation</t>
   </si>
   <si>
-    <t>IRI or CURI for this vocabulary</t>
-  </si>
-  <si>
     <t>Title of the vocabulary</t>
   </si>
   <si>
@@ -273,12 +276,18 @@
     <t>Concept Scheme*</t>
   </si>
   <si>
+    <t>ex:test_</t>
+  </si>
+  <si>
     <t>Test-of-Voc4Cat</t>
   </si>
   <si>
     <t>A test vocabulary for the voc4cat template</t>
   </si>
   <si>
+    <t>ex:c01</t>
+  </si>
+  <si>
     <t>en</t>
   </si>
   <si>
@@ -286,6 +295,9 @@
   </si>
   <si>
     <t>https://www.w3.org/TR/2010/NOTE-curie-20101216/</t>
+  </si>
+  <si>
+    <t>ex:c02</t>
   </si>
   <si>
     <t>URI</t>
@@ -325,7 +337,19 @@
     <t>IRI</t>
   </si>
   <si>
+    <t>ex:c03</t>
+  </si>
+  <si>
+    <t>ex:col1</t>
+  </si>
+  <si>
     <t>Linked data term</t>
+  </si>
+  <si>
+    <t>ex:c01, ex:c02, ex:c03</t>
+  </si>
+  <si>
+    <t>voc4cat-template</t>
   </si>
   <si>
     <t>Collection of term related to linked data.</t>
@@ -409,6 +433,9 @@
   </si>
   <si>
     <t>If you need help, feel free to create issues on github for your questions.</t>
+  </si>
+  <si>
+    <t>v2023-03-10</t>
   </si>
   <si>
     <t>Version specifier for the vocabulary</t>
@@ -1537,34 +1564,16 @@
     <t>Concepts*</t>
   </si>
   <si>
-    <t>2023-06a</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0001-2345-6789 Sofia Garcia</t>
-  </si>
-  <si>
-    <t>v2023-07-25</t>
-  </si>
-  <si>
-    <t>exvoc</t>
-  </si>
-  <si>
-    <t>https://example.org/exvoc</t>
-  </si>
-  <si>
-    <t>exvoc:0000001</t>
-  </si>
-  <si>
-    <t>exvoc:0000002</t>
-  </si>
-  <si>
-    <t>exvoc:0000003</t>
-  </si>
-  <si>
-    <t>exvoc:0000010</t>
-  </si>
-  <si>
-    <t>exvoc:0000001, exvoc:0000002, exvoc:0000003</t>
+    <t>https://w3id.org/nfdi4cat/voc4cat_</t>
+  </si>
+  <si>
+    <t>2023-07a</t>
+  </si>
+  <si>
+    <t>IRI or CURIE for this vocabulary</t>
+  </si>
+  <si>
+    <t>Required: URI or CURIE</t>
   </si>
 </sst>
 </file>
@@ -2460,9 +2469,7 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2479,7 +2486,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2488,15 +2495,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2557,31 +2564,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2589,29 +2596,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2646,12 +2653,12 @@
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2719,7 +2726,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2732,10 +2739,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2745,10 +2752,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2769,7 +2776,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3144,7 +3151,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3598,7 +3605,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3898,7 +3905,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -4055,7 +4062,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4179,7 +4186,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4236,18 +4243,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5329,7 +5336,7 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5338,12 +5345,12 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="64.140625" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5351,13 +5358,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -5365,10 +5372,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5379,10 +5386,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5396,10 +5403,10 @@
         <v>44995</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5407,13 +5414,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="16">
-        <v>45132</v>
+        <v>44995</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5424,10 +5431,10 @@
         <v>29</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5438,10 +5445,10 @@
         <v>29</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -5449,10 +5456,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -5463,7 +5470,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>12</v>
@@ -5477,7 +5484,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -6494,7 +6501,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6512,7 +6519,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6523,19 +6530,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -6546,86 +6553,80 @@
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>80</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>64</v>
-      </c>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="H5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
@@ -6635,7 +6636,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="17"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6794,7 +6795,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -6813,7 +6814,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6824,7 +6825,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6832,27 +6833,27 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
@@ -7354,7 +7355,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7373,7 +7374,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -7382,27 +7383,27 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>107</v>
+        <v>84</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7538,10 +7539,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7562,15 +7563,23 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -7581,11 +7590,12 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://example.org/new/" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat/" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Template: example data updated to pass validation
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333FB821-20CB-452C-9828-FF39C2B47E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F6358D-99C9-4DF5-8A5B-42C5AF07ECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="119">
   <si>
     <t>0.4.3</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Namespace</t>
   </si>
   <si>
-    <t>ex</t>
-  </si>
-  <si>
     <t>NFDI4Cat</t>
   </si>
   <si>
@@ -195,18 +192,9 @@
     <t>https://github.com/nfdi4cat/vocexcel</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>voc4cat</t>
   </si>
   <si>
-    <t>https://example.org/</t>
-  </si>
-  <si>
-    <t>https://example.org/new/</t>
-  </si>
-  <si>
     <t>The spreadsheet is processed with voc4cat which extends vocexcel for the voc4cat-based repositories.</t>
   </si>
   <si>
@@ -276,18 +264,12 @@
     <t>Concept Scheme*</t>
   </si>
   <si>
-    <t>ex:test_</t>
-  </si>
-  <si>
     <t>Test-of-Voc4Cat</t>
   </si>
   <si>
     <t>A test vocabulary for the voc4cat template</t>
   </si>
   <si>
-    <t>ex:c01</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -295,9 +277,6 @@
   </si>
   <si>
     <t>https://www.w3.org/TR/2010/NOTE-curie-20101216/</t>
-  </si>
-  <si>
-    <t>ex:c02</t>
   </si>
   <si>
     <t>URI</t>
@@ -337,22 +316,7 @@
     <t>IRI</t>
   </si>
   <si>
-    <t>ex:c03</t>
-  </si>
-  <si>
-    <t>ex:col1</t>
-  </si>
-  <si>
     <t>Linked data term</t>
-  </si>
-  <si>
-    <t>ex:c01, ex:c02, ex:c03</t>
-  </si>
-  <si>
-    <t>voc4cat-template</t>
-  </si>
-  <si>
-    <t>Collection of term related to linked data.</t>
   </si>
   <si>
     <t>https://datatracker.ietf.org/doc/html/rfc3987</t>
@@ -435,9 +399,6 @@
     <t>If you need help, feel free to create issues on github for your questions.</t>
   </si>
   <si>
-    <t>v2023-03-10</t>
-  </si>
-  <si>
     <t>Version specifier for the vocabulary</t>
   </si>
   <si>
@@ -635,12 +596,34 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Collections (optional)</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Finally...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alteratively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prefix Sheet</t>
     </r>
     <r>
       <rPr>
@@ -663,135 +646,135 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Collections are an easy way to group together concepts for various purposes.
-If rows are added to the sheet, all cells must be filled out.
+      <t>This sheet is for defining a mapping between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
+Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "http://example.org/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" as the coresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
 </t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Preferred Label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A simple one-line title for the Collection.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Definition</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The defining description of this Collection that may be longer and include line-breaks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ember IRIs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A comma-separated list of the Concept IRIS of all Concepts belonging to this collection.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provenance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A note on the source of this Collection</t>
-    </r>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE a colon is used to seperate the prefix from the suffix-part of the IRI.</t>
+    </r>
+  </si>
+  <si>
+    <t>revision</t>
+  </si>
+  <si>
+    <t>Concepts*</t>
+  </si>
+  <si>
+    <t>https://w3id.org/nfdi4cat/voc4cat_</t>
+  </si>
+  <si>
+    <t>IRI or CURIE for this vocabulary</t>
+  </si>
+  <si>
+    <t>Required: URI or CURIE</t>
+  </si>
+  <si>
+    <t>0000-0001-2345-6789 Created concept</t>
+  </si>
+  <si>
+    <t>https://example.org/test/</t>
+  </si>
+  <si>
+    <t>ext</t>
+  </si>
+  <si>
+    <t>ext:0000002</t>
+  </si>
+  <si>
+    <t>ext:0000003</t>
+  </si>
+  <si>
+    <t>ext:0000001</t>
+  </si>
+  <si>
+    <t>ext:0000010</t>
+  </si>
+  <si>
+    <t>ext:0000001, ext:0000002, ext:0000003</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-2345-6789 Sofia Garcia</t>
+  </si>
+  <si>
+    <t>ext:</t>
+  </si>
+  <si>
+    <t>Collection of terms related to linked data.</t>
+  </si>
+  <si>
+    <t>v2023-08-11</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-2345-6789 Created collection</t>
+  </si>
+  <si>
+    <t>2023-08a</t>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Finally...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alteratively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1085,7 +1068,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = A note on the source of this vocabulary.
+      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a github name should be used. Multiple entries must be seperated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
 </t>
     </r>
     <r>
@@ -1131,109 +1114,6 @@
       </rPr>
       <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prefix Sheet</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This sheet is for defining a mapping between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
-Example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "http://example.org/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" as the coresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE a colon is used to seperate the prefix from the suffix-part of the IRI.</t>
-    </r>
-  </si>
-  <si>
-    <t>revision</t>
   </si>
   <si>
     <r>
@@ -1527,7 +1407,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = A note on the source of this Concept
+      <t xml:space="preserve"> = A note on the source of this Concept; see above for what is expected in provenance fields.
 </t>
     </r>
     <r>
@@ -1561,19 +1441,139 @@
     </r>
   </si>
   <si>
-    <t>Concepts*</t>
-  </si>
-  <si>
-    <t>https://w3id.org/nfdi4cat/voc4cat_</t>
-  </si>
-  <si>
-    <t>2023-07a</t>
-  </si>
-  <si>
-    <t>IRI or CURIE for this vocabulary</t>
-  </si>
-  <si>
-    <t>Required: URI or CURIE</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Collections (optional)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Collections are an easy way to group together concepts for various purposes.
+If rows are added to the sheet, all cells must be filled out.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Preferred Label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A simple one-line title for the Collection.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Definition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The defining description of this Collection that may be longer and include line-breaks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ember IRIs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A comma-separated list of the Concept IRIS of all Concepts belonging to this collection.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provenance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A note on the source of this Collection; see above for what is expected in provenance fields.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2157,8 +2157,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B20" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:B20" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B19" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:B19" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A30D4DF8-3B4A-4F43-9882-EDFDD8090F9E}" name="Prefix"/>
     <tableColumn id="2" xr3:uid="{6285A3D9-0152-4BE7-AC6A-AF758EEFAF51}" name="Namespace"/>
@@ -2469,7 +2469,9 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2486,7 +2488,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2495,15 +2497,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2564,31 +2566,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2596,29 +2598,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2653,12 +2655,12 @@
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2726,7 +2728,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2739,10 +2741,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2752,10 +2754,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2776,7 +2778,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3151,7 +3153,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3605,7 +3607,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3905,7 +3907,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -4062,7 +4064,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4186,7 +4188,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4243,18 +4245,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5337,7 +5339,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5350,7 +5352,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5358,13 +5360,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>61</v>
+        <v>111</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -5372,10 +5374,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5386,10 +5388,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5403,10 +5405,10 @@
         <v>44995</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5414,13 +5416,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="16">
-        <v>44995</v>
+        <v>45149</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5428,13 +5430,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5442,13 +5444,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -5456,10 +5458,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -5470,7 +5472,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>12</v>
@@ -5484,7 +5486,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -6519,7 +6521,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6530,19 +6532,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -6553,80 +6555,86 @@
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="9"/>
+        <v>102</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="9"/>
+        <v>102</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
@@ -6795,7 +6803,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{4A3F3B18-10F7-4667-9E5E-AD9B1C4C3B42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -6825,7 +6833,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6833,27 +6841,27 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
@@ -7355,7 +7363,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7374,7 +7382,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -7383,27 +7391,27 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7539,10 +7547,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7560,42 +7568,33 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Prefix ends with colon" error="A prefix may not end with a colon(:)!" sqref="A2:A20" xr:uid="{3E636239-7DFF-4815-80F6-149A9A69419E}">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Prefix ends with colon" error="A prefix may not end with a colon(:)!" sqref="A2:A19" xr:uid="{3E636239-7DFF-4815-80F6-149A9A69419E}">
       <formula1>ISERROR(SEARCH(":",A2))</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{721C34C9-12AA-45FE-91A4-8BCB1AB59BCB}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat/" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://w3id.org/nfdi4cat/voc4cat/" xr:uid="{0E392E66-5F6B-4692-BC52-7DAF5D46D4EA}"/>
+    <hyperlink ref="B2" r:id="rId2" display="https://example.org/" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update workflows for 0.7.0 & new release workflow
Includes template update for now optional version & modified date
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F6358D-99C9-4DF5-8A5B-42C5AF07ECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F32D2C7-B0FD-4E9C-80DE-890B9DBC774A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
   <si>
     <t>0.4.3</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Created Date*</t>
   </si>
   <si>
-    <t>Modified Date*</t>
-  </si>
-  <si>
     <t>Creator*</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Vocabulary Content Manager</t>
   </si>
   <si>
-    <t>Optional</t>
-  </si>
-  <si>
     <t>Catalogue PID</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>examples of filled-out templates</t>
   </si>
   <si>
-    <t>https://surroundaustralia.github.io/vocpub-profile/specification.html</t>
-  </si>
-  <si>
     <t>SKOS RDF data produced or consumed by with voc4cat are validated against the VocPub profile using SHACL.</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
   </si>
   <si>
     <t>Required: Date</t>
-  </si>
-  <si>
-    <t>Date of last modification</t>
   </si>
   <si>
     <t>Date of creation</t>
@@ -399,9 +387,6 @@
     <t>If you need help, feel free to create issues on github for your questions.</t>
   </si>
   <si>
-    <t>Version specifier for the vocabulary</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -766,354 +751,6 @@
   </si>
   <si>
     <t>https://orcid.org/0000-0001-2345-6789 Created collection</t>
-  </si>
-  <si>
-    <t>2023-08a</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Concept Scheme (mandatory)</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Vocabulary IRI* </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= The IRI tat refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replae it later (e.g. http://example.com/def/v1 ). 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on te Prefix Sheet.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  A short one line title for the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Created Date*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's creation date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Modified Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's latest modification date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Creator*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The ID of an organisation e.g. "GA". 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Publisher*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The ID of an organisation e.g. "CGI".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Either the abbreviation for an organisation or its full name can be given. The organisation is validated against a predefined list of organisations. If you miss an organisation, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based vesioning)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provenance*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a github name should be used. Multiple entries must be seperated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Custodian</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Catalogue PID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1574,6 +1211,394 @@
       </rPr>
       <t xml:space="preserve"> = A note on the source of this Collection; see above for what is expected in provenance fields.</t>
     </r>
+  </si>
+  <si>
+    <t>2023-08b</t>
+  </si>
+  <si>
+    <t>https://w3id.org/profile/vocpub</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concept Scheme (mandatory)</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Vocabulary IRI* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= The IRI tat refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replae it later (e.g. http://example.com/def/v1 ). 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on te Prefix Sheet.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  A short one line title for the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Created Date*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's creation date.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modified Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's latest modification date (optional).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creator*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Publisher*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Either the abbreviation for an organisation or its URI can be given. The organisation abbreviation is validated against a predefined list of organisations. If you miss an organisation, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based vesioning).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Versions strings should start with "v" to prevent Excel from interpreting it as number of date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provenance*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a github name should be used. Multiple entries must be seperated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Custodian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Catalogue PID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional: Date</t>
+  </si>
+  <si>
+    <t>Version specifier for the vocabulary (or empty cell)</t>
+  </si>
+  <si>
+    <t>Date of last modification (or empty cell)</t>
+  </si>
+  <si>
+    <t>Modified Date</t>
+  </si>
+  <si>
+    <t>Optional: URI or Text</t>
   </si>
 </sst>
 </file>
@@ -2488,7 +2513,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2497,15 +2522,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2566,31 +2591,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2598,29 +2623,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2646,21 +2671,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1170"/>
+  <dimension ref="A1:J1172"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:J88"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2728,7 +2755,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2741,10 +2768,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2754,10 +2781,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2778,7 +2805,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3142,19 +3169,18 @@
       <c r="J44" s="27"/>
     </row>
     <row r="45" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="27" t="s">
-        <v>117</v>
-      </c>
+      <c r="B46" s="27"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
@@ -3165,18 +3191,19 @@
       <c r="J46" s="27"/>
     </row>
     <row r="47" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
+      <c r="B48" s="27" t="s">
+        <v>110</v>
+      </c>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
@@ -3604,11 +3631,19 @@
       <c r="I86" s="27"/>
       <c r="J86" s="27"/>
     </row>
-    <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
+      <c r="J87" s="27"/>
+    </row>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B88" s="27" t="s">
-        <v>94</v>
-      </c>
+      <c r="B88" s="27"/>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
       <c r="E88" s="27"/>
@@ -3618,19 +3653,11 @@
       <c r="I88" s="27"/>
       <c r="J88" s="27"/>
     </row>
-    <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-    </row>
+    <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B90" s="27"/>
+      <c r="B90" s="27" t="s">
+        <v>89</v>
+      </c>
       <c r="C90" s="27"/>
       <c r="D90" s="27"/>
       <c r="E90" s="27"/>
@@ -3904,11 +3931,19 @@
       <c r="I114" s="27"/>
       <c r="J114" s="27"/>
     </row>
-    <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B115" s="27"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27"/>
+      <c r="H115" s="27"/>
+      <c r="I115" s="27"/>
+      <c r="J115" s="27"/>
+    </row>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B116" s="27" t="s">
-        <v>118</v>
-      </c>
+      <c r="B116" s="27"/>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
       <c r="E116" s="27"/>
@@ -3918,19 +3953,11 @@
       <c r="I116" s="27"/>
       <c r="J116" s="27"/>
     </row>
-    <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B117" s="27"/>
-      <c r="C117" s="27"/>
-      <c r="D117" s="27"/>
-      <c r="E117" s="27"/>
-      <c r="F117" s="27"/>
-      <c r="G117" s="27"/>
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
-      <c r="J117" s="27"/>
-    </row>
+    <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B118" s="27"/>
+      <c r="B118" s="27" t="s">
+        <v>111</v>
+      </c>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
       <c r="E118" s="27"/>
@@ -4061,11 +4088,19 @@
       <c r="I129" s="27"/>
       <c r="J129" s="27"/>
     </row>
-    <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B130" s="27"/>
+      <c r="C130" s="27"/>
+      <c r="D130" s="27"/>
+      <c r="E130" s="27"/>
+      <c r="F130" s="27"/>
+      <c r="G130" s="27"/>
+      <c r="H130" s="27"/>
+      <c r="I130" s="27"/>
+      <c r="J130" s="27"/>
+    </row>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B131" s="27" t="s">
-        <v>96</v>
-      </c>
+      <c r="B131" s="27"/>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
       <c r="E131" s="27"/>
@@ -4075,19 +4110,11 @@
       <c r="I131" s="27"/>
       <c r="J131" s="27"/>
     </row>
-    <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B132" s="27"/>
-      <c r="C132" s="27"/>
-      <c r="D132" s="27"/>
-      <c r="E132" s="27"/>
-      <c r="F132" s="27"/>
-      <c r="G132" s="27"/>
-      <c r="H132" s="27"/>
-      <c r="I132" s="27"/>
-      <c r="J132" s="27"/>
-    </row>
+    <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B133" s="27"/>
+      <c r="B133" s="27" t="s">
+        <v>91</v>
+      </c>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
       <c r="E133" s="27"/>
@@ -4185,33 +4212,33 @@
       <c r="I141" s="27"/>
       <c r="J141" s="27"/>
     </row>
-    <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B142" s="27"/>
+      <c r="C142" s="27"/>
+      <c r="D142" s="27"/>
+      <c r="E142" s="27"/>
+      <c r="F142" s="27"/>
+      <c r="G142" s="27"/>
+      <c r="H142" s="27"/>
+      <c r="I142" s="27"/>
+      <c r="J142" s="27"/>
+    </row>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B143" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C143" s="28"/>
-      <c r="D143" s="28"/>
-      <c r="E143" s="28"/>
-      <c r="F143" s="28"/>
-      <c r="G143" s="28"/>
-      <c r="H143" s="28"/>
-      <c r="I143" s="28"/>
-      <c r="J143" s="28"/>
-    </row>
-    <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B144" s="28"/>
-      <c r="C144" s="28"/>
-      <c r="D144" s="28"/>
-      <c r="E144" s="28"/>
-      <c r="F144" s="28"/>
-      <c r="G144" s="28"/>
-      <c r="H144" s="28"/>
-      <c r="I144" s="28"/>
-      <c r="J144" s="28"/>
-    </row>
+      <c r="B143" s="27"/>
+      <c r="C143" s="27"/>
+      <c r="D143" s="27"/>
+      <c r="E143" s="27"/>
+      <c r="F143" s="27"/>
+      <c r="G143" s="27"/>
+      <c r="H143" s="27"/>
+      <c r="I143" s="27"/>
+      <c r="J143" s="27"/>
+    </row>
+    <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B145" s="28"/>
+      <c r="B145" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
       <c r="E145" s="28"/>
@@ -4244,23 +4271,43 @@
       <c r="J147" s="28"/>
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D148" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E148" s="10" t="s">
-        <v>87</v>
-      </c>
+      <c r="B148" s="28"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="28"/>
+      <c r="E148" s="28"/>
+      <c r="F148" s="28"/>
+      <c r="G148" s="28"/>
+      <c r="H148" s="28"/>
+      <c r="I148" s="28"/>
+      <c r="J148" s="28"/>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D149" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E149" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+      <c r="B149" s="28"/>
+      <c r="C149" s="28"/>
+      <c r="D149" s="28"/>
+      <c r="E149" s="28"/>
+      <c r="F149" s="28"/>
+      <c r="G149" s="28"/>
+      <c r="H149" s="28"/>
+      <c r="I149" s="28"/>
+      <c r="J149" s="28"/>
+    </row>
+    <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D150" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E150" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D151" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E151" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="152" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="153" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="154" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5280,51 +5327,53 @@
     <row r="1168" ht="15" x14ac:dyDescent="0.25"/>
     <row r="1169" ht="15" x14ac:dyDescent="0.25"/>
     <row r="1170" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="1171" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="1172" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B131:J141"/>
-    <mergeCell ref="B143:J147"/>
+    <mergeCell ref="B133:J143"/>
+    <mergeCell ref="B145:J149"/>
     <mergeCell ref="B2:J6"/>
-    <mergeCell ref="B12:J44"/>
-    <mergeCell ref="B46:J86"/>
-    <mergeCell ref="B88:J114"/>
-    <mergeCell ref="B116:J129"/>
+    <mergeCell ref="B12:J46"/>
+    <mergeCell ref="B48:J88"/>
+    <mergeCell ref="B90:J116"/>
+    <mergeCell ref="B118:J131"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B4 B46:B86">
+  <conditionalFormatting sqref="B2:B4 B48:B88">
     <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B44">
+  <conditionalFormatting sqref="B12:B46">
     <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B88">
+  <conditionalFormatting sqref="B90">
     <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(B88))=0</formula>
+      <formula>LEN(TRIM(B90))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B116">
+  <conditionalFormatting sqref="B118">
     <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(B116))=0</formula>
+      <formula>LEN(TRIM(B118))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B131">
+  <conditionalFormatting sqref="B133">
     <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(B131))=0</formula>
+      <formula>LEN(TRIM(B133))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B143:B147">
+  <conditionalFormatting sqref="B145:B149">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B143))=0</formula>
+      <formula>LEN(TRIM(B145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{57547A46-992F-4B46-8DCE-6851DE974B0D}"/>
     <hyperlink ref="D9" r:id="rId2" xr:uid="{7DDFAC11-0287-4E46-9BC5-4CE195DD88F1}"/>
-    <hyperlink ref="E149" r:id="rId3" xr:uid="{A5C8A041-9B1E-4C57-A8AC-D56D5CF97571}"/>
-    <hyperlink ref="E148" r:id="rId4" xr:uid="{7FFAD8C3-AA0B-4A81-9A4D-A7DC6B7D6670}"/>
+    <hyperlink ref="E151" r:id="rId3" xr:uid="{A5C8A041-9B1E-4C57-A8AC-D56D5CF97571}"/>
+    <hyperlink ref="E150" r:id="rId4" xr:uid="{7FFAD8C3-AA0B-4A81-9A4D-A7DC6B7D6670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -5339,7 +5388,7 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5352,7 +5401,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5360,13 +5409,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -5374,10 +5423,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5388,10 +5437,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5405,77 +5454,77 @@
         <v>44995</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="B6" s="16">
         <v>45149</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>12</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>3</v>
@@ -5483,28 +5532,28 @@
     </row>
     <row r="11" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="D11" s="14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
@@ -6521,119 +6570,119 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -6833,35 +6882,35 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
@@ -7377,41 +7426,41 @@
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7560,26 +7609,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to Python 3.13 and voc4cat-tool to v0.10.0
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-template\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A839B1AC-B4BB-4F71-8F64-ED9B5C07F92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB75596-3025-4802-AC9E-EF43E3547A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28260" windowHeight="11265" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
   <si>
     <t>Template version</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>revision</t>
-  </si>
-  <si>
-    <t>2025-02a</t>
   </si>
   <si>
     <t>This spreadsheet is a template for creating and maintaining vocabularies for linked open data. With the help of the Python package voc4cat linked below, the information in this spreadsheet can be converted into SKOS RDF files (e.g. in turtle format). The other direction is also possible: An empty template may be filled with the information from a compatible SKOS RDF data file. So SKOS data can be edited using a spreadsheet program as user interface. The column names in this template closely mirror the terms in the SKOS data model.</t>
@@ -370,9 +367,6 @@
     <t>Alternate Labels</t>
   </si>
   <si>
-    <t>Children IRIs</t>
-  </si>
-  <si>
     <t>Source Vocab URI</t>
   </si>
   <si>
@@ -500,6 +494,21 @@
   </si>
   <si>
     <t>https://example.org/</t>
+  </si>
+  <si>
+    <t>Parent IRIs</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>0.4.3, rev. 2025-07a</t>
+  </si>
+  <si>
+    <t>Version of the xlsx template</t>
+  </si>
+  <si>
+    <t>2025-07a</t>
   </si>
 </sst>
 </file>
@@ -704,7 +713,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -797,6 +806,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -957,7 +967,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Definition*"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Def. Language Code"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Alternate Labels"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Children IRIs"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parent IRIs"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Provenance*"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Source Vocab URI"/>
   </tableColumns>
@@ -1307,7 +1317,9 @@
   </sheetPr>
   <dimension ref="A11:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1336,105 +1348,105 @@
         <v>2</v>
       </c>
       <c r="J12" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="37" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
       <c r="L16" s="12"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
       <c r="L17" s="12"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="33" t="s">
         <v>6</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="26" t="s">
         <v>8</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>10</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="26" t="s">
         <v>12</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1442,29 +1454,29 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>14</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D28" s="13"/>
       <c r="E28" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D32" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1500,65 +1512,65 @@
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -1573,7 +1585,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1586,10 +1598,10 @@
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16"/>
       <c r="C9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>24</v>
       </c>
       <c r="F9" s="34"/>
       <c r="G9" s="1"/>
@@ -1599,10 +1611,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>26</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="1"/>
@@ -1622,391 +1634,391 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
+      <c r="B12" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
     </row>
     <row r="37" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
     </row>
     <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
     </row>
     <row r="43" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
     </row>
     <row r="46" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
@@ -2019,1081 +2031,1081 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
+      <c r="B48" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="37"/>
-      <c r="J51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="38"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="37"/>
-      <c r="J52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
     </row>
     <row r="53" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
     </row>
     <row r="54" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
     </row>
     <row r="55" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
-      <c r="J55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
     </row>
     <row r="56" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="37"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="37"/>
-      <c r="J56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
     </row>
     <row r="57" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
     </row>
     <row r="58" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
     </row>
     <row r="59" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
+      <c r="J59" s="38"/>
     </row>
     <row r="60" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
-      <c r="D60" s="37"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="37"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="37"/>
-      <c r="J60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
     </row>
     <row r="61" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="37"/>
-      <c r="J61" s="37"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="38"/>
     </row>
     <row r="62" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="37"/>
-      <c r="I62" s="37"/>
-      <c r="J62" s="37"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="38"/>
     </row>
     <row r="63" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="37"/>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
     </row>
     <row r="64" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="37"/>
-      <c r="I64" s="37"/>
-      <c r="J64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
     </row>
     <row r="65" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="37"/>
-      <c r="J65" s="37"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
     </row>
     <row r="66" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="37"/>
-      <c r="H66" s="37"/>
-      <c r="I66" s="37"/>
-      <c r="J66" s="37"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
     </row>
     <row r="67" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="37"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
     </row>
     <row r="68" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
-      <c r="I68" s="37"/>
-      <c r="J68" s="37"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
     </row>
     <row r="69" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="37"/>
-      <c r="I69" s="37"/>
-      <c r="J69" s="37"/>
+      <c r="B69" s="38"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
     </row>
     <row r="70" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="37"/>
-      <c r="H70" s="37"/>
-      <c r="I70" s="37"/>
-      <c r="J70" s="37"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
     </row>
     <row r="71" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="37"/>
+      <c r="B71" s="38"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
     </row>
     <row r="72" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="37"/>
-      <c r="I72" s="37"/>
-      <c r="J72" s="37"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="38"/>
     </row>
     <row r="73" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="37"/>
-      <c r="H73" s="37"/>
-      <c r="I73" s="37"/>
-      <c r="J73" s="37"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
     </row>
     <row r="74" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="37"/>
-      <c r="H74" s="37"/>
-      <c r="I74" s="37"/>
-      <c r="J74" s="37"/>
+      <c r="B74" s="38"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+      <c r="J74" s="38"/>
     </row>
     <row r="75" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="37"/>
-      <c r="G75" s="37"/>
-      <c r="H75" s="37"/>
-      <c r="I75" s="37"/>
-      <c r="J75" s="37"/>
+      <c r="B75" s="38"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
+      <c r="J75" s="38"/>
     </row>
     <row r="76" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="37"/>
-      <c r="I76" s="37"/>
-      <c r="J76" s="37"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="38"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
+      <c r="J76" s="38"/>
     </row>
     <row r="77" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="37"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="37"/>
-      <c r="I77" s="37"/>
-      <c r="J77" s="37"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
     </row>
     <row r="78" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="37"/>
-      <c r="I78" s="37"/>
-      <c r="J78" s="37"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="38"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="38"/>
     </row>
     <row r="79" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="37"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="37"/>
-      <c r="H79" s="37"/>
-      <c r="I79" s="37"/>
-      <c r="J79" s="37"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
     </row>
     <row r="80" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="37"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="37"/>
-      <c r="H80" s="37"/>
-      <c r="I80" s="37"/>
-      <c r="J80" s="37"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="38"/>
     </row>
     <row r="81" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="37"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="37"/>
-      <c r="G81" s="37"/>
-      <c r="H81" s="37"/>
-      <c r="I81" s="37"/>
-      <c r="J81" s="37"/>
+      <c r="B81" s="38"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="38"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="38"/>
+      <c r="I81" s="38"/>
+      <c r="J81" s="38"/>
     </row>
     <row r="82" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="37"/>
-      <c r="H82" s="37"/>
-      <c r="I82" s="37"/>
-      <c r="J82" s="37"/>
+      <c r="B82" s="38"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="38"/>
+      <c r="J82" s="38"/>
     </row>
     <row r="83" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="37"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="37"/>
-      <c r="I83" s="37"/>
-      <c r="J83" s="37"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="38"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="38"/>
+      <c r="J83" s="38"/>
     </row>
     <row r="84" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="37"/>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="37"/>
-      <c r="I84" s="37"/>
-      <c r="J84" s="37"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="38"/>
     </row>
     <row r="85" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="37"/>
-      <c r="H85" s="37"/>
-      <c r="I85" s="37"/>
-      <c r="J85" s="37"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="38"/>
     </row>
     <row r="86" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="37"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="37"/>
-      <c r="H86" s="37"/>
-      <c r="I86" s="37"/>
-      <c r="J86" s="37"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="38"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="38"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="38"/>
+      <c r="J86" s="38"/>
     </row>
     <row r="87" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="37"/>
-      <c r="H87" s="37"/>
-      <c r="I87" s="37"/>
-      <c r="J87" s="37"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="38"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
     </row>
     <row r="88" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="37"/>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
-      <c r="G88" s="37"/>
-      <c r="H88" s="37"/>
-      <c r="I88" s="37"/>
-      <c r="J88" s="37"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="38"/>
     </row>
     <row r="89" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
-      <c r="G90" s="37"/>
-      <c r="H90" s="37"/>
-      <c r="I90" s="37"/>
-      <c r="J90" s="37"/>
+      <c r="B90" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="38"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="38"/>
     </row>
     <row r="91" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="37"/>
-      <c r="C91" s="37"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
-      <c r="G91" s="37"/>
-      <c r="H91" s="37"/>
-      <c r="I91" s="37"/>
-      <c r="J91" s="37"/>
+      <c r="B91" s="38"/>
+      <c r="C91" s="38"/>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="38"/>
+      <c r="J91" s="38"/>
     </row>
     <row r="92" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="37"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="37"/>
-      <c r="G92" s="37"/>
-      <c r="H92" s="37"/>
-      <c r="I92" s="37"/>
-      <c r="J92" s="37"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="38"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="38"/>
+      <c r="J92" s="38"/>
     </row>
     <row r="93" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="37"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
-      <c r="G93" s="37"/>
-      <c r="H93" s="37"/>
-      <c r="I93" s="37"/>
-      <c r="J93" s="37"/>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="38"/>
+      <c r="H93" s="38"/>
+      <c r="I93" s="38"/>
+      <c r="J93" s="38"/>
     </row>
     <row r="94" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="37"/>
-      <c r="H94" s="37"/>
-      <c r="I94" s="37"/>
-      <c r="J94" s="37"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="38"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="38"/>
+      <c r="H94" s="38"/>
+      <c r="I94" s="38"/>
+      <c r="J94" s="38"/>
     </row>
     <row r="95" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="37"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
-      <c r="G95" s="37"/>
-      <c r="H95" s="37"/>
-      <c r="I95" s="37"/>
-      <c r="J95" s="37"/>
+      <c r="B95" s="38"/>
+      <c r="C95" s="38"/>
+      <c r="D95" s="38"/>
+      <c r="E95" s="38"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="38"/>
+      <c r="H95" s="38"/>
+      <c r="I95" s="38"/>
+      <c r="J95" s="38"/>
     </row>
     <row r="96" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="37"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="37"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="37"/>
-      <c r="G96" s="37"/>
-      <c r="H96" s="37"/>
-      <c r="I96" s="37"/>
-      <c r="J96" s="37"/>
+      <c r="B96" s="38"/>
+      <c r="C96" s="38"/>
+      <c r="D96" s="38"/>
+      <c r="E96" s="38"/>
+      <c r="F96" s="38"/>
+      <c r="G96" s="38"/>
+      <c r="H96" s="38"/>
+      <c r="I96" s="38"/>
+      <c r="J96" s="38"/>
     </row>
     <row r="97" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="37"/>
-      <c r="C97" s="37"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="37"/>
-      <c r="I97" s="37"/>
-      <c r="J97" s="37"/>
+      <c r="B97" s="38"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="38"/>
+      <c r="E97" s="38"/>
+      <c r="F97" s="38"/>
+      <c r="G97" s="38"/>
+      <c r="H97" s="38"/>
+      <c r="I97" s="38"/>
+      <c r="J97" s="38"/>
     </row>
     <row r="98" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="37"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="37"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="37"/>
-      <c r="G98" s="37"/>
-      <c r="H98" s="37"/>
-      <c r="I98" s="37"/>
-      <c r="J98" s="37"/>
+      <c r="B98" s="38"/>
+      <c r="C98" s="38"/>
+      <c r="D98" s="38"/>
+      <c r="E98" s="38"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="38"/>
+      <c r="H98" s="38"/>
+      <c r="I98" s="38"/>
+      <c r="J98" s="38"/>
     </row>
     <row r="99" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="37"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
-      <c r="G99" s="37"/>
-      <c r="H99" s="37"/>
-      <c r="I99" s="37"/>
-      <c r="J99" s="37"/>
+      <c r="B99" s="38"/>
+      <c r="C99" s="38"/>
+      <c r="D99" s="38"/>
+      <c r="E99" s="38"/>
+      <c r="F99" s="38"/>
+      <c r="G99" s="38"/>
+      <c r="H99" s="38"/>
+      <c r="I99" s="38"/>
+      <c r="J99" s="38"/>
     </row>
     <row r="100" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="37"/>
-      <c r="C100" s="37"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="37"/>
-      <c r="H100" s="37"/>
-      <c r="I100" s="37"/>
-      <c r="J100" s="37"/>
+      <c r="B100" s="38"/>
+      <c r="C100" s="38"/>
+      <c r="D100" s="38"/>
+      <c r="E100" s="38"/>
+      <c r="F100" s="38"/>
+      <c r="G100" s="38"/>
+      <c r="H100" s="38"/>
+      <c r="I100" s="38"/>
+      <c r="J100" s="38"/>
     </row>
     <row r="101" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="37"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="37"/>
-      <c r="H101" s="37"/>
-      <c r="I101" s="37"/>
-      <c r="J101" s="37"/>
+      <c r="B101" s="38"/>
+      <c r="C101" s="38"/>
+      <c r="D101" s="38"/>
+      <c r="E101" s="38"/>
+      <c r="F101" s="38"/>
+      <c r="G101" s="38"/>
+      <c r="H101" s="38"/>
+      <c r="I101" s="38"/>
+      <c r="J101" s="38"/>
     </row>
     <row r="102" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="37"/>
-      <c r="C102" s="37"/>
-      <c r="D102" s="37"/>
-      <c r="E102" s="37"/>
-      <c r="F102" s="37"/>
-      <c r="G102" s="37"/>
-      <c r="H102" s="37"/>
-      <c r="I102" s="37"/>
-      <c r="J102" s="37"/>
+      <c r="B102" s="38"/>
+      <c r="C102" s="38"/>
+      <c r="D102" s="38"/>
+      <c r="E102" s="38"/>
+      <c r="F102" s="38"/>
+      <c r="G102" s="38"/>
+      <c r="H102" s="38"/>
+      <c r="I102" s="38"/>
+      <c r="J102" s="38"/>
     </row>
     <row r="103" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="37"/>
-      <c r="C103" s="37"/>
-      <c r="D103" s="37"/>
-      <c r="E103" s="37"/>
-      <c r="F103" s="37"/>
-      <c r="G103" s="37"/>
-      <c r="H103" s="37"/>
-      <c r="I103" s="37"/>
-      <c r="J103" s="37"/>
+      <c r="B103" s="38"/>
+      <c r="C103" s="38"/>
+      <c r="D103" s="38"/>
+      <c r="E103" s="38"/>
+      <c r="F103" s="38"/>
+      <c r="G103" s="38"/>
+      <c r="H103" s="38"/>
+      <c r="I103" s="38"/>
+      <c r="J103" s="38"/>
     </row>
     <row r="104" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="37"/>
-      <c r="C104" s="37"/>
-      <c r="D104" s="37"/>
-      <c r="E104" s="37"/>
-      <c r="F104" s="37"/>
-      <c r="G104" s="37"/>
-      <c r="H104" s="37"/>
-      <c r="I104" s="37"/>
-      <c r="J104" s="37"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="38"/>
+      <c r="D104" s="38"/>
+      <c r="E104" s="38"/>
+      <c r="F104" s="38"/>
+      <c r="G104" s="38"/>
+      <c r="H104" s="38"/>
+      <c r="I104" s="38"/>
+      <c r="J104" s="38"/>
     </row>
     <row r="105" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="37"/>
-      <c r="C105" s="37"/>
-      <c r="D105" s="37"/>
-      <c r="E105" s="37"/>
-      <c r="F105" s="37"/>
-      <c r="G105" s="37"/>
-      <c r="H105" s="37"/>
-      <c r="I105" s="37"/>
-      <c r="J105" s="37"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
+      <c r="G105" s="38"/>
+      <c r="H105" s="38"/>
+      <c r="I105" s="38"/>
+      <c r="J105" s="38"/>
     </row>
     <row r="106" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="37"/>
-      <c r="C106" s="37"/>
-      <c r="D106" s="37"/>
-      <c r="E106" s="37"/>
-      <c r="F106" s="37"/>
-      <c r="G106" s="37"/>
-      <c r="H106" s="37"/>
-      <c r="I106" s="37"/>
-      <c r="J106" s="37"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="38"/>
+      <c r="D106" s="38"/>
+      <c r="E106" s="38"/>
+      <c r="F106" s="38"/>
+      <c r="G106" s="38"/>
+      <c r="H106" s="38"/>
+      <c r="I106" s="38"/>
+      <c r="J106" s="38"/>
     </row>
     <row r="107" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="37"/>
-      <c r="C107" s="37"/>
-      <c r="D107" s="37"/>
-      <c r="E107" s="37"/>
-      <c r="F107" s="37"/>
-      <c r="G107" s="37"/>
-      <c r="H107" s="37"/>
-      <c r="I107" s="37"/>
-      <c r="J107" s="37"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="38"/>
+      <c r="D107" s="38"/>
+      <c r="E107" s="38"/>
+      <c r="F107" s="38"/>
+      <c r="G107" s="38"/>
+      <c r="H107" s="38"/>
+      <c r="I107" s="38"/>
+      <c r="J107" s="38"/>
     </row>
     <row r="108" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="37"/>
-      <c r="C108" s="37"/>
-      <c r="D108" s="37"/>
-      <c r="E108" s="37"/>
-      <c r="F108" s="37"/>
-      <c r="G108" s="37"/>
-      <c r="H108" s="37"/>
-      <c r="I108" s="37"/>
-      <c r="J108" s="37"/>
+      <c r="B108" s="38"/>
+      <c r="C108" s="38"/>
+      <c r="D108" s="38"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="38"/>
+      <c r="H108" s="38"/>
+      <c r="I108" s="38"/>
+      <c r="J108" s="38"/>
     </row>
     <row r="109" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="37"/>
-      <c r="C109" s="37"/>
-      <c r="D109" s="37"/>
-      <c r="E109" s="37"/>
-      <c r="F109" s="37"/>
-      <c r="G109" s="37"/>
-      <c r="H109" s="37"/>
-      <c r="I109" s="37"/>
-      <c r="J109" s="37"/>
+      <c r="B109" s="38"/>
+      <c r="C109" s="38"/>
+      <c r="D109" s="38"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
+      <c r="G109" s="38"/>
+      <c r="H109" s="38"/>
+      <c r="I109" s="38"/>
+      <c r="J109" s="38"/>
     </row>
     <row r="110" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="37"/>
-      <c r="C110" s="37"/>
-      <c r="D110" s="37"/>
-      <c r="E110" s="37"/>
-      <c r="F110" s="37"/>
-      <c r="G110" s="37"/>
-      <c r="H110" s="37"/>
-      <c r="I110" s="37"/>
-      <c r="J110" s="37"/>
+      <c r="B110" s="38"/>
+      <c r="C110" s="38"/>
+      <c r="D110" s="38"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
+      <c r="G110" s="38"/>
+      <c r="H110" s="38"/>
+      <c r="I110" s="38"/>
+      <c r="J110" s="38"/>
     </row>
     <row r="111" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="37"/>
-      <c r="C111" s="37"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="37"/>
-      <c r="F111" s="37"/>
-      <c r="G111" s="37"/>
-      <c r="H111" s="37"/>
-      <c r="I111" s="37"/>
-      <c r="J111" s="37"/>
+      <c r="B111" s="38"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="38"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
+      <c r="I111" s="38"/>
+      <c r="J111" s="38"/>
     </row>
     <row r="112" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="37"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="37"/>
-      <c r="E112" s="37"/>
-      <c r="F112" s="37"/>
-      <c r="G112" s="37"/>
-      <c r="H112" s="37"/>
-      <c r="I112" s="37"/>
-      <c r="J112" s="37"/>
+      <c r="B112" s="38"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
+      <c r="J112" s="38"/>
     </row>
     <row r="113" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="37"/>
-      <c r="C113" s="37"/>
-      <c r="D113" s="37"/>
-      <c r="E113" s="37"/>
-      <c r="F113" s="37"/>
-      <c r="G113" s="37"/>
-      <c r="H113" s="37"/>
-      <c r="I113" s="37"/>
-      <c r="J113" s="37"/>
+      <c r="B113" s="38"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="38"/>
+      <c r="E113" s="38"/>
+      <c r="F113" s="38"/>
+      <c r="G113" s="38"/>
+      <c r="H113" s="38"/>
+      <c r="I113" s="38"/>
+      <c r="J113" s="38"/>
     </row>
     <row r="114" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="37"/>
-      <c r="C114" s="37"/>
-      <c r="D114" s="37"/>
-      <c r="E114" s="37"/>
-      <c r="F114" s="37"/>
-      <c r="G114" s="37"/>
-      <c r="H114" s="37"/>
-      <c r="I114" s="37"/>
-      <c r="J114" s="37"/>
+      <c r="B114" s="38"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38"/>
+      <c r="E114" s="38"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="38"/>
+      <c r="H114" s="38"/>
+      <c r="I114" s="38"/>
+      <c r="J114" s="38"/>
     </row>
     <row r="115" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="37"/>
-      <c r="C115" s="37"/>
-      <c r="D115" s="37"/>
-      <c r="E115" s="37"/>
-      <c r="F115" s="37"/>
-      <c r="G115" s="37"/>
-      <c r="H115" s="37"/>
-      <c r="I115" s="37"/>
-      <c r="J115" s="37"/>
+      <c r="B115" s="38"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38"/>
+      <c r="E115" s="38"/>
+      <c r="F115" s="38"/>
+      <c r="G115" s="38"/>
+      <c r="H115" s="38"/>
+      <c r="I115" s="38"/>
+      <c r="J115" s="38"/>
     </row>
     <row r="116" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="37"/>
-      <c r="C116" s="37"/>
-      <c r="D116" s="37"/>
-      <c r="E116" s="37"/>
-      <c r="F116" s="37"/>
-      <c r="G116" s="37"/>
-      <c r="H116" s="37"/>
-      <c r="I116" s="37"/>
-      <c r="J116" s="37"/>
+      <c r="B116" s="38"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
+      <c r="G116" s="38"/>
+      <c r="H116" s="38"/>
+      <c r="I116" s="38"/>
+      <c r="J116" s="38"/>
     </row>
     <row r="117" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C118" s="37"/>
-      <c r="D118" s="37"/>
-      <c r="E118" s="37"/>
-      <c r="F118" s="37"/>
-      <c r="G118" s="37"/>
-      <c r="H118" s="37"/>
-      <c r="I118" s="37"/>
-      <c r="J118" s="37"/>
+      <c r="B118" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" s="38"/>
+      <c r="D118" s="38"/>
+      <c r="E118" s="38"/>
+      <c r="F118" s="38"/>
+      <c r="G118" s="38"/>
+      <c r="H118" s="38"/>
+      <c r="I118" s="38"/>
+      <c r="J118" s="38"/>
     </row>
     <row r="119" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="37"/>
-      <c r="C119" s="37"/>
-      <c r="D119" s="37"/>
-      <c r="E119" s="37"/>
-      <c r="F119" s="37"/>
-      <c r="G119" s="37"/>
-      <c r="H119" s="37"/>
-      <c r="I119" s="37"/>
-      <c r="J119" s="37"/>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38"/>
+      <c r="E119" s="38"/>
+      <c r="F119" s="38"/>
+      <c r="G119" s="38"/>
+      <c r="H119" s="38"/>
+      <c r="I119" s="38"/>
+      <c r="J119" s="38"/>
     </row>
     <row r="120" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="37"/>
-      <c r="C120" s="37"/>
-      <c r="D120" s="37"/>
-      <c r="E120" s="37"/>
-      <c r="F120" s="37"/>
-      <c r="G120" s="37"/>
-      <c r="H120" s="37"/>
-      <c r="I120" s="37"/>
-      <c r="J120" s="37"/>
+      <c r="B120" s="38"/>
+      <c r="C120" s="38"/>
+      <c r="D120" s="38"/>
+      <c r="E120" s="38"/>
+      <c r="F120" s="38"/>
+      <c r="G120" s="38"/>
+      <c r="H120" s="38"/>
+      <c r="I120" s="38"/>
+      <c r="J120" s="38"/>
     </row>
     <row r="121" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="37"/>
-      <c r="C121" s="37"/>
-      <c r="D121" s="37"/>
-      <c r="E121" s="37"/>
-      <c r="F121" s="37"/>
-      <c r="G121" s="37"/>
-      <c r="H121" s="37"/>
-      <c r="I121" s="37"/>
-      <c r="J121" s="37"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="38"/>
+      <c r="D121" s="38"/>
+      <c r="E121" s="38"/>
+      <c r="F121" s="38"/>
+      <c r="G121" s="38"/>
+      <c r="H121" s="38"/>
+      <c r="I121" s="38"/>
+      <c r="J121" s="38"/>
     </row>
     <row r="122" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="37"/>
-      <c r="C122" s="37"/>
-      <c r="D122" s="37"/>
-      <c r="E122" s="37"/>
-      <c r="F122" s="37"/>
-      <c r="G122" s="37"/>
-      <c r="H122" s="37"/>
-      <c r="I122" s="37"/>
-      <c r="J122" s="37"/>
+      <c r="B122" s="38"/>
+      <c r="C122" s="38"/>
+      <c r="D122" s="38"/>
+      <c r="E122" s="38"/>
+      <c r="F122" s="38"/>
+      <c r="G122" s="38"/>
+      <c r="H122" s="38"/>
+      <c r="I122" s="38"/>
+      <c r="J122" s="38"/>
     </row>
     <row r="123" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="37"/>
-      <c r="C123" s="37"/>
-      <c r="D123" s="37"/>
-      <c r="E123" s="37"/>
-      <c r="F123" s="37"/>
-      <c r="G123" s="37"/>
-      <c r="H123" s="37"/>
-      <c r="I123" s="37"/>
-      <c r="J123" s="37"/>
+      <c r="B123" s="38"/>
+      <c r="C123" s="38"/>
+      <c r="D123" s="38"/>
+      <c r="E123" s="38"/>
+      <c r="F123" s="38"/>
+      <c r="G123" s="38"/>
+      <c r="H123" s="38"/>
+      <c r="I123" s="38"/>
+      <c r="J123" s="38"/>
     </row>
     <row r="124" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="37"/>
-      <c r="C124" s="37"/>
-      <c r="D124" s="37"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="37"/>
-      <c r="H124" s="37"/>
-      <c r="I124" s="37"/>
-      <c r="J124" s="37"/>
+      <c r="B124" s="38"/>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38"/>
+      <c r="E124" s="38"/>
+      <c r="F124" s="38"/>
+      <c r="G124" s="38"/>
+      <c r="H124" s="38"/>
+      <c r="I124" s="38"/>
+      <c r="J124" s="38"/>
     </row>
     <row r="125" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="37"/>
-      <c r="C125" s="37"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="37"/>
-      <c r="G125" s="37"/>
-      <c r="H125" s="37"/>
-      <c r="I125" s="37"/>
-      <c r="J125" s="37"/>
+      <c r="B125" s="38"/>
+      <c r="C125" s="38"/>
+      <c r="D125" s="38"/>
+      <c r="E125" s="38"/>
+      <c r="F125" s="38"/>
+      <c r="G125" s="38"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="38"/>
+      <c r="J125" s="38"/>
     </row>
     <row r="126" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="37"/>
-      <c r="C126" s="37"/>
-      <c r="D126" s="37"/>
-      <c r="E126" s="37"/>
-      <c r="F126" s="37"/>
-      <c r="G126" s="37"/>
-      <c r="H126" s="37"/>
-      <c r="I126" s="37"/>
-      <c r="J126" s="37"/>
+      <c r="B126" s="38"/>
+      <c r="C126" s="38"/>
+      <c r="D126" s="38"/>
+      <c r="E126" s="38"/>
+      <c r="F126" s="38"/>
+      <c r="G126" s="38"/>
+      <c r="H126" s="38"/>
+      <c r="I126" s="38"/>
+      <c r="J126" s="38"/>
     </row>
     <row r="127" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="37"/>
-      <c r="C127" s="37"/>
-      <c r="D127" s="37"/>
-      <c r="E127" s="37"/>
-      <c r="F127" s="37"/>
-      <c r="G127" s="37"/>
-      <c r="H127" s="37"/>
-      <c r="I127" s="37"/>
-      <c r="J127" s="37"/>
+      <c r="B127" s="38"/>
+      <c r="C127" s="38"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="38"/>
+      <c r="F127" s="38"/>
+      <c r="G127" s="38"/>
+      <c r="H127" s="38"/>
+      <c r="I127" s="38"/>
+      <c r="J127" s="38"/>
     </row>
     <row r="128" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="37"/>
-      <c r="C128" s="37"/>
-      <c r="D128" s="37"/>
-      <c r="E128" s="37"/>
-      <c r="F128" s="37"/>
-      <c r="G128" s="37"/>
-      <c r="H128" s="37"/>
-      <c r="I128" s="37"/>
-      <c r="J128" s="37"/>
+      <c r="B128" s="38"/>
+      <c r="C128" s="38"/>
+      <c r="D128" s="38"/>
+      <c r="E128" s="38"/>
+      <c r="F128" s="38"/>
+      <c r="G128" s="38"/>
+      <c r="H128" s="38"/>
+      <c r="I128" s="38"/>
+      <c r="J128" s="38"/>
     </row>
     <row r="129" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="37"/>
-      <c r="C129" s="37"/>
-      <c r="D129" s="37"/>
-      <c r="E129" s="37"/>
-      <c r="F129" s="37"/>
-      <c r="G129" s="37"/>
-      <c r="H129" s="37"/>
-      <c r="I129" s="37"/>
-      <c r="J129" s="37"/>
+      <c r="B129" s="38"/>
+      <c r="C129" s="38"/>
+      <c r="D129" s="38"/>
+      <c r="E129" s="38"/>
+      <c r="F129" s="38"/>
+      <c r="G129" s="38"/>
+      <c r="H129" s="38"/>
+      <c r="I129" s="38"/>
+      <c r="J129" s="38"/>
     </row>
     <row r="130" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="37"/>
-      <c r="C130" s="37"/>
-      <c r="D130" s="37"/>
-      <c r="E130" s="37"/>
-      <c r="F130" s="37"/>
-      <c r="G130" s="37"/>
-      <c r="H130" s="37"/>
-      <c r="I130" s="37"/>
-      <c r="J130" s="37"/>
+      <c r="B130" s="38"/>
+      <c r="C130" s="38"/>
+      <c r="D130" s="38"/>
+      <c r="E130" s="38"/>
+      <c r="F130" s="38"/>
+      <c r="G130" s="38"/>
+      <c r="H130" s="38"/>
+      <c r="I130" s="38"/>
+      <c r="J130" s="38"/>
     </row>
     <row r="131" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="37"/>
-      <c r="C131" s="37"/>
-      <c r="D131" s="37"/>
-      <c r="E131" s="37"/>
-      <c r="F131" s="37"/>
-      <c r="G131" s="37"/>
-      <c r="H131" s="37"/>
-      <c r="I131" s="37"/>
-      <c r="J131" s="37"/>
+      <c r="B131" s="38"/>
+      <c r="C131" s="38"/>
+      <c r="D131" s="38"/>
+      <c r="E131" s="38"/>
+      <c r="F131" s="38"/>
+      <c r="G131" s="38"/>
+      <c r="H131" s="38"/>
+      <c r="I131" s="38"/>
+      <c r="J131" s="38"/>
     </row>
     <row r="132" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C133" s="37"/>
-      <c r="D133" s="37"/>
-      <c r="E133" s="37"/>
-      <c r="F133" s="37"/>
-      <c r="G133" s="37"/>
-      <c r="H133" s="37"/>
-      <c r="I133" s="37"/>
-      <c r="J133" s="37"/>
+      <c r="B133" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C133" s="38"/>
+      <c r="D133" s="38"/>
+      <c r="E133" s="38"/>
+      <c r="F133" s="38"/>
+      <c r="G133" s="38"/>
+      <c r="H133" s="38"/>
+      <c r="I133" s="38"/>
+      <c r="J133" s="38"/>
     </row>
     <row r="134" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="37"/>
-      <c r="C134" s="37"/>
-      <c r="D134" s="37"/>
-      <c r="E134" s="37"/>
-      <c r="F134" s="37"/>
-      <c r="G134" s="37"/>
-      <c r="H134" s="37"/>
-      <c r="I134" s="37"/>
-      <c r="J134" s="37"/>
+      <c r="B134" s="38"/>
+      <c r="C134" s="38"/>
+      <c r="D134" s="38"/>
+      <c r="E134" s="38"/>
+      <c r="F134" s="38"/>
+      <c r="G134" s="38"/>
+      <c r="H134" s="38"/>
+      <c r="I134" s="38"/>
+      <c r="J134" s="38"/>
     </row>
     <row r="135" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="37"/>
-      <c r="C135" s="37"/>
-      <c r="D135" s="37"/>
-      <c r="E135" s="37"/>
-      <c r="F135" s="37"/>
-      <c r="G135" s="37"/>
-      <c r="H135" s="37"/>
-      <c r="I135" s="37"/>
-      <c r="J135" s="37"/>
+      <c r="B135" s="38"/>
+      <c r="C135" s="38"/>
+      <c r="D135" s="38"/>
+      <c r="E135" s="38"/>
+      <c r="F135" s="38"/>
+      <c r="G135" s="38"/>
+      <c r="H135" s="38"/>
+      <c r="I135" s="38"/>
+      <c r="J135" s="38"/>
     </row>
     <row r="136" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="37"/>
-      <c r="C136" s="37"/>
-      <c r="D136" s="37"/>
-      <c r="E136" s="37"/>
-      <c r="F136" s="37"/>
-      <c r="G136" s="37"/>
-      <c r="H136" s="37"/>
-      <c r="I136" s="37"/>
-      <c r="J136" s="37"/>
+      <c r="B136" s="38"/>
+      <c r="C136" s="38"/>
+      <c r="D136" s="38"/>
+      <c r="E136" s="38"/>
+      <c r="F136" s="38"/>
+      <c r="G136" s="38"/>
+      <c r="H136" s="38"/>
+      <c r="I136" s="38"/>
+      <c r="J136" s="38"/>
     </row>
     <row r="137" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="37"/>
-      <c r="C137" s="37"/>
-      <c r="D137" s="37"/>
-      <c r="E137" s="37"/>
-      <c r="F137" s="37"/>
-      <c r="G137" s="37"/>
-      <c r="H137" s="37"/>
-      <c r="I137" s="37"/>
-      <c r="J137" s="37"/>
+      <c r="B137" s="38"/>
+      <c r="C137" s="38"/>
+      <c r="D137" s="38"/>
+      <c r="E137" s="38"/>
+      <c r="F137" s="38"/>
+      <c r="G137" s="38"/>
+      <c r="H137" s="38"/>
+      <c r="I137" s="38"/>
+      <c r="J137" s="38"/>
     </row>
     <row r="138" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="37"/>
-      <c r="C138" s="37"/>
-      <c r="D138" s="37"/>
-      <c r="E138" s="37"/>
-      <c r="F138" s="37"/>
-      <c r="G138" s="37"/>
-      <c r="H138" s="37"/>
-      <c r="I138" s="37"/>
-      <c r="J138" s="37"/>
+      <c r="B138" s="38"/>
+      <c r="C138" s="38"/>
+      <c r="D138" s="38"/>
+      <c r="E138" s="38"/>
+      <c r="F138" s="38"/>
+      <c r="G138" s="38"/>
+      <c r="H138" s="38"/>
+      <c r="I138" s="38"/>
+      <c r="J138" s="38"/>
     </row>
     <row r="139" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="37"/>
-      <c r="C139" s="37"/>
-      <c r="D139" s="37"/>
-      <c r="E139" s="37"/>
-      <c r="F139" s="37"/>
-      <c r="G139" s="37"/>
-      <c r="H139" s="37"/>
-      <c r="I139" s="37"/>
-      <c r="J139" s="37"/>
+      <c r="B139" s="38"/>
+      <c r="C139" s="38"/>
+      <c r="D139" s="38"/>
+      <c r="E139" s="38"/>
+      <c r="F139" s="38"/>
+      <c r="G139" s="38"/>
+      <c r="H139" s="38"/>
+      <c r="I139" s="38"/>
+      <c r="J139" s="38"/>
     </row>
     <row r="140" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="37"/>
-      <c r="C140" s="37"/>
-      <c r="D140" s="37"/>
-      <c r="E140" s="37"/>
-      <c r="F140" s="37"/>
-      <c r="G140" s="37"/>
-      <c r="H140" s="37"/>
-      <c r="I140" s="37"/>
-      <c r="J140" s="37"/>
+      <c r="B140" s="38"/>
+      <c r="C140" s="38"/>
+      <c r="D140" s="38"/>
+      <c r="E140" s="38"/>
+      <c r="F140" s="38"/>
+      <c r="G140" s="38"/>
+      <c r="H140" s="38"/>
+      <c r="I140" s="38"/>
+      <c r="J140" s="38"/>
     </row>
     <row r="141" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="37"/>
-      <c r="C141" s="37"/>
-      <c r="D141" s="37"/>
-      <c r="E141" s="37"/>
-      <c r="F141" s="37"/>
-      <c r="G141" s="37"/>
-      <c r="H141" s="37"/>
-      <c r="I141" s="37"/>
-      <c r="J141" s="37"/>
+      <c r="B141" s="38"/>
+      <c r="C141" s="38"/>
+      <c r="D141" s="38"/>
+      <c r="E141" s="38"/>
+      <c r="F141" s="38"/>
+      <c r="G141" s="38"/>
+      <c r="H141" s="38"/>
+      <c r="I141" s="38"/>
+      <c r="J141" s="38"/>
     </row>
     <row r="142" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C143" s="37"/>
-      <c r="D143" s="37"/>
-      <c r="E143" s="37"/>
-      <c r="F143" s="37"/>
-      <c r="G143" s="37"/>
-      <c r="H143" s="37"/>
-      <c r="I143" s="37"/>
-      <c r="J143" s="37"/>
+      <c r="B143" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C143" s="38"/>
+      <c r="D143" s="38"/>
+      <c r="E143" s="38"/>
+      <c r="F143" s="38"/>
+      <c r="G143" s="38"/>
+      <c r="H143" s="38"/>
+      <c r="I143" s="38"/>
+      <c r="J143" s="38"/>
     </row>
     <row r="144" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="37"/>
-      <c r="C144" s="37"/>
-      <c r="D144" s="37"/>
-      <c r="E144" s="37"/>
-      <c r="F144" s="37"/>
-      <c r="G144" s="37"/>
-      <c r="H144" s="37"/>
-      <c r="I144" s="37"/>
-      <c r="J144" s="37"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="38"/>
+      <c r="D144" s="38"/>
+      <c r="E144" s="38"/>
+      <c r="F144" s="38"/>
+      <c r="G144" s="38"/>
+      <c r="H144" s="38"/>
+      <c r="I144" s="38"/>
+      <c r="J144" s="38"/>
     </row>
     <row r="145" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="37"/>
-      <c r="C145" s="37"/>
-      <c r="D145" s="37"/>
-      <c r="E145" s="37"/>
-      <c r="F145" s="37"/>
-      <c r="G145" s="37"/>
-      <c r="H145" s="37"/>
-      <c r="I145" s="37"/>
-      <c r="J145" s="37"/>
+      <c r="B145" s="38"/>
+      <c r="C145" s="38"/>
+      <c r="D145" s="38"/>
+      <c r="E145" s="38"/>
+      <c r="F145" s="38"/>
+      <c r="G145" s="38"/>
+      <c r="H145" s="38"/>
+      <c r="I145" s="38"/>
+      <c r="J145" s="38"/>
     </row>
     <row r="146" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="37"/>
-      <c r="C146" s="37"/>
-      <c r="D146" s="37"/>
-      <c r="E146" s="37"/>
-      <c r="F146" s="37"/>
-      <c r="G146" s="37"/>
-      <c r="H146" s="37"/>
-      <c r="I146" s="37"/>
-      <c r="J146" s="37"/>
+      <c r="B146" s="38"/>
+      <c r="C146" s="38"/>
+      <c r="D146" s="38"/>
+      <c r="E146" s="38"/>
+      <c r="F146" s="38"/>
+      <c r="G146" s="38"/>
+      <c r="H146" s="38"/>
+      <c r="I146" s="38"/>
+      <c r="J146" s="38"/>
     </row>
     <row r="147" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="37"/>
-      <c r="C147" s="37"/>
-      <c r="D147" s="37"/>
-      <c r="E147" s="37"/>
-      <c r="F147" s="37"/>
-      <c r="G147" s="37"/>
-      <c r="H147" s="37"/>
-      <c r="I147" s="37"/>
-      <c r="J147" s="37"/>
+      <c r="B147" s="38"/>
+      <c r="C147" s="38"/>
+      <c r="D147" s="38"/>
+      <c r="E147" s="38"/>
+      <c r="F147" s="38"/>
+      <c r="G147" s="38"/>
+      <c r="H147" s="38"/>
+      <c r="I147" s="38"/>
+      <c r="J147" s="38"/>
     </row>
     <row r="148" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D148" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E148" s="34" t="s">
         <v>33</v>
-      </c>
-      <c r="E148" s="34" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4172,10 +4184,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D994"/>
+  <dimension ref="A1:D995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4188,162 +4200,175 @@
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="C5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="C9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="13" spans="1:4" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5325,6 +5350,7 @@
     <row r="992" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{23038B36-221D-493D-8F66-BDC6E25D7069}"/>
@@ -5342,7 +5368,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5360,119 +5386,119 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C2" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F2" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="23" t="s">
         <v>78</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="D3" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="E3" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>83</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="E4" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="G4" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="27" t="s">
+      <c r="H4" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="30" t="s">
         <v>91</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="E5" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>95</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>97</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -5522,35 +5548,35 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="F2" s="23" t="s">
         <v>102</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
@@ -6032,41 +6058,41 @@
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="D3" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="E3" s="25" t="s">
         <v>115</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6107,18 +6133,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update template for ParentIRIs coming with v0.10.0
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCFAF9A-16AB-4F1A-9E10-106FA17068AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76FE9C2-B719-4322-A919-24F5CE758CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="8700" windowWidth="28500" windowHeight="8535" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28260" windowHeight="16380" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
   <si>
     <t>Template version</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Alternate Labels</t>
   </si>
   <si>
-    <t>Children IRIs</t>
-  </si>
-  <si>
     <t>Source Vocab URI</t>
   </si>
   <si>
@@ -285,9 +282,6 @@
   </si>
   <si>
     <t>Namespace</t>
-  </si>
-  <si>
-    <t>2025-02a</t>
   </si>
   <si>
     <t>Voc4Cat online help &amp; guidelines</t>
@@ -493,7 +487,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Concepts (mandatory)</t>
+      <t>Prefix Sheet</t>
     </r>
     <r>
       <rPr>
@@ -516,6 +510,688 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>This sheet shows the known mappings between short prefixes and namespaces which are the basis for using "compact URI" also called "CURIE". This sheet is write only; any changes will be ignored. For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
+Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "http://example.org/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Finally...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alternatively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concept Scheme (mandatory)</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Vocabulary IRI* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= The IRI that refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replace it later (e.g. http://example.com/def/v1 ). 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on the Prefix Sheet.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  A short one line title for the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Created Date*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's creation date.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modified Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's latest modification date (optional).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creator*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Publisher*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Either the abbreviation for an organization or its URI can be given. The organization abbreviation is validated against a predefined list of organizations. If you miss an organization, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based versioning).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Versions strings should start with "v" to prevent Excel from interpreting it as number of date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provenance*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a GitHub name should be used. Multiple entries must be separated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Custodian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Catalogue PID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
+    </r>
+  </si>
+  <si>
+    <t>2025-07a</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t>0.4.3, rev. 2025-07a</t>
+  </si>
+  <si>
+    <t>Version of the xlsx template</t>
+  </si>
+  <si>
+    <t>Parent IRIs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Additional Concept Features (optional)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The Additional Concept Features sheet allows to add more relations between concepts. These extra relations are adapted from the SKOS specification.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: In this sheet you can also use CURIEs instead of full IRIs using the mappings defined in the prefix sheet. In all *-Matches columns multiple concept-IRIs (or CURIEs) can be entered as comma-separated list.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concept IRI*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The concept IRI as defined in sheet Concepts.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Related Matches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = This cell asserts a related or associated relationship between the concepts listed. It's important to note that these concepts aren't close enough to be transitive.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Close Matches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Mapping with this cell means the concepts are sufficiently similar that they can be used interchangeably. However, these concepts are not close enough to be transitive amongst each other.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exact Matches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = This is a subset of a close match. Concepts are to be added if they are similar enough to be used interchangeably but have an even higher degree of closeness that includes transitivity. e.g. if example 1 is an exact match of example 2, and example 2 is an exact match of example 3, it follows example 1 is an exact match of example 3.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Broader Matches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Broader match allows the user to assert that a concept is broader in meaning to another concept. e.g. a strawberry has a broader concept of fruit. This is the inverse of a narrower property. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Narrower Matches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Narrower match allows the user to assert a concept is narrower in meaning to another concept. e.g. fruit has a narrower concept of strawberries. This is the inverse of a broader property.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note on Broader/Narrower: In sheet "Concepts" broader/narrower is expressed via "Parent IRIs". The broader/narrower columns in this sheet should be used to express broader/narrower relations with external concepts.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concepts (mandatory)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">A concept according to SKOS is a unit of thought, idea, meaning, or category of an object or event which underlies a knowledge organization system. This sheet collects concept descriptions, (optionally) their translations to other languages, simple broader/ narrower relations between the concepts and provenance information.
 </t>
     </r>
@@ -605,7 +1281,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> = Two or three letter language code according to ISO 639-2 or 639-3 for the Preferred Label  (see https://iso639-3.sil.org/code_tables/639/data).  If no language code is given, "en" is assumed as default.
-With voc4cat you may use indentation of the Preferred Label (xlsx-indentation or character-based indentation) to express parent-child (broader/narrower) relations between concepts. If you use indentation, the Children IRIs column (see below) is ignored. voc4cat allows to convert in both directions between indentation-based and Children-IRIs-based representation.
 </t>
     </r>
     <r>
@@ -726,16 +1401,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Children URIs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A list of IRIs of children of this Concept, separated by commas. This creates a hierarchical relationship between the terms. In SKOS terminology, the Concept is broader than its Concept-Child and in turn the Concept-Child is narrower than the Concept. </t>
+      <t>Parent IRIs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A list of IRIs of parents of this Concept, separated by commas. This creates a hierarchical relationship between the terms. In SKOS terminology, the Concept is narrower than its Concept-Parent and in turn the Concept-Parent is broader than the Concept. </t>
     </r>
     <r>
       <rPr>
@@ -806,673 +1481,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Additional Concept Features (optional)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The Additional Concept Features sheet allows to add more relations between concepts. These extra relations are adapted from the SKOS specification.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: In this sheet you can also use CURIEs instead of full IRIs using the mappings defined in the prefix sheet. In all *-Matches columns multiple concept-IRIs (or CURIEs) can be entered as comma-separated list.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Concept IRI*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The concept IRI as defined in sheet Concepts.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Related Matches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = This cell asserts a related or associated relationship between the concepts listed. It's important to note that these concepts aren't close enough to be transitive.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Close Matches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Mapping with this cell means the concepts are sufficiently similar that they can be used interchangeably. However, these concepts are not close enough to be transitive amongst each other.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exact Matches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = This is a subset of a close match. Concepts are to be added if they are similar enough to be used interchangeably but have an even higher degree of closeness that includes transitivity. e.g. if example 1 is an exact match of example 2, and example 2 is an exact match of example 3, it follows example 1 is an exact match of example 3.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Broader Matches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Broader match allows the user to assert that a concept is broader in meaning to another concept. e.g. a strawberry has a broader concept of fruit. This is the inverse of a narrower property. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Narrower Matches</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Narrower match allows the user to assert a concept is narrower in meaning to another concept. e.g. fruit has a narrower concept of strawberries. This is the inverse of a broader property.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note on Broader/Narrower: In sheet "Concepts" broader/narrower is expressed via "Children URIs" or as indentation. The broader/narrower columns in this sheet should be used to express broader/narrower relations with external concepts.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prefix Sheet</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This sheet shows the known mappings between short prefixes and namespaces which are the basis for using "compact URI" also called "CURIE". This sheet is write only; any changes will be ignored. For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
-Example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "http://example.org/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Finally...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alternatively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Concept Scheme (mandatory)</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Vocabulary IRI* </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= The IRI that refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replace it later (e.g. http://example.com/def/v1 ). 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on the Prefix Sheet.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  A short one line title for the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Created Date*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's creation date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Modified Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's latest modification date (optional).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Creator*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Publisher*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Either the abbreviation for an organization or its URI can be given. The organization abbreviation is validated against a predefined list of organizations. If you miss an organization, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based versioning).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Versions strings should start with "v" to prevent Excel from interpreting it as number of date.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provenance*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a GitHub name should be used. Multiple entries must be separated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Custodian</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Catalogue PID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
     </r>
   </si>
 </sst>
@@ -1739,7 +1747,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1830,6 +1838,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1993,7 +2002,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Definition*"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Def. Language Code"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Alternate Labels"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Children IRIs"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parent IRIs"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Provenance*"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Source Vocab URI" dataDxfId="6"/>
   </tableColumns>
@@ -2343,7 +2352,9 @@
   </sheetPr>
   <dimension ref="A11:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2372,86 +2383,86 @@
         <v>2</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
+      <c r="B14" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
       <c r="L16" s="12"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
       <c r="L17" s="12"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D22" s="33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D23" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>3</v>
@@ -2459,18 +2470,18 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2540,61 +2551,61 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -2609,7 +2620,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2658,391 +2669,391 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
+      <c r="B12" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
     </row>
     <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
     </row>
     <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
     </row>
     <row r="23" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
     </row>
     <row r="25" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
     </row>
     <row r="26" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
     </row>
     <row r="27" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
     </row>
     <row r="32" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
     </row>
     <row r="33" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
     </row>
     <row r="34" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
     </row>
     <row r="35" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="37"/>
     </row>
     <row r="36" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
     </row>
     <row r="37" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
     </row>
     <row r="38" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
     </row>
     <row r="39" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
     </row>
     <row r="40" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
     </row>
     <row r="41" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
     </row>
     <row r="42" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
     </row>
     <row r="44" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="37"/>
     </row>
     <row r="45" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
@@ -3055,1074 +3066,1074 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="36"/>
+      <c r="B48" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
     </row>
     <row r="49" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
     </row>
     <row r="50" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="36"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
     </row>
     <row r="51" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
     </row>
     <row r="52" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
     </row>
     <row r="53" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="36"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
     </row>
     <row r="54" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="36"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
     </row>
     <row r="55" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
     </row>
     <row r="56" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
     </row>
     <row r="57" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
     </row>
     <row r="58" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="36"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
     </row>
     <row r="59" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
     </row>
     <row r="60" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="36"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
     </row>
     <row r="61" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
     </row>
     <row r="62" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="36"/>
-      <c r="J62" s="36"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
     </row>
     <row r="63" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="36"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
     </row>
     <row r="64" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
     </row>
     <row r="65" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="36"/>
-      <c r="I65" s="36"/>
-      <c r="J65" s="36"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
     </row>
     <row r="66" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="36"/>
-      <c r="I66" s="36"/>
-      <c r="J66" s="36"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
     </row>
     <row r="67" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="36"/>
-      <c r="J67" s="36"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
     </row>
     <row r="68" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="36"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
     </row>
     <row r="69" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="36"/>
-      <c r="I69" s="36"/>
-      <c r="J69" s="36"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
     </row>
     <row r="70" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
-      <c r="J70" s="36"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
     </row>
     <row r="71" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="36"/>
-      <c r="J71" s="36"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
     </row>
     <row r="72" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="36"/>
-      <c r="J72" s="36"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
     </row>
     <row r="73" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="36"/>
-      <c r="J73" s="36"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
     </row>
     <row r="74" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B74" s="36"/>
-      <c r="C74" s="36"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
     </row>
     <row r="75" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B75" s="36"/>
-      <c r="C75" s="36"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="36"/>
-      <c r="G75" s="36"/>
-      <c r="H75" s="36"/>
-      <c r="I75" s="36"/>
-      <c r="J75" s="36"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
     </row>
     <row r="76" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="36"/>
-      <c r="I76" s="36"/>
-      <c r="J76" s="36"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
     </row>
     <row r="77" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="36"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="36"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="37"/>
     </row>
     <row r="78" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="36"/>
-      <c r="I78" s="36"/>
-      <c r="J78" s="36"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="37"/>
     </row>
     <row r="79" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="36"/>
-      <c r="G79" s="36"/>
-      <c r="H79" s="36"/>
-      <c r="I79" s="36"/>
-      <c r="J79" s="36"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
     </row>
     <row r="80" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B80" s="36"/>
-      <c r="C80" s="36"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="36"/>
-      <c r="H80" s="36"/>
-      <c r="I80" s="36"/>
-      <c r="J80" s="36"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="37"/>
     </row>
     <row r="81" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="36"/>
-      <c r="I81" s="36"/>
-      <c r="J81" s="36"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37"/>
+      <c r="I81" s="37"/>
+      <c r="J81" s="37"/>
     </row>
     <row r="82" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B82" s="36"/>
-      <c r="C82" s="36"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="36"/>
-      <c r="G82" s="36"/>
-      <c r="H82" s="36"/>
-      <c r="I82" s="36"/>
-      <c r="J82" s="36"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
     </row>
     <row r="83" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B83" s="36"/>
-      <c r="C83" s="36"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="36"/>
-      <c r="G83" s="36"/>
-      <c r="H83" s="36"/>
-      <c r="I83" s="36"/>
-      <c r="J83" s="36"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37"/>
     </row>
     <row r="84" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="36"/>
-      <c r="I84" s="36"/>
-      <c r="J84" s="36"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37"/>
+      <c r="J84" s="37"/>
     </row>
     <row r="85" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="36"/>
-      <c r="I85" s="36"/>
-      <c r="J85" s="36"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="37"/>
     </row>
     <row r="86" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B86" s="36"/>
-      <c r="C86" s="36"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="36"/>
-      <c r="I86" s="36"/>
-      <c r="J86" s="36"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
     </row>
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B87" s="36"/>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="36"/>
-      <c r="G87" s="36"/>
-      <c r="H87" s="36"/>
-      <c r="I87" s="36"/>
-      <c r="J87" s="36"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="37"/>
     </row>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B88" s="36"/>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36"/>
-      <c r="H88" s="36"/>
-      <c r="I88" s="36"/>
-      <c r="J88" s="36"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="37"/>
     </row>
     <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B90" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C90" s="36"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36"/>
-      <c r="F90" s="36"/>
-      <c r="G90" s="36"/>
-      <c r="H90" s="36"/>
-      <c r="I90" s="36"/>
-      <c r="J90" s="36"/>
+      <c r="B90" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="37"/>
+      <c r="J90" s="37"/>
     </row>
     <row r="91" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B91" s="36"/>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="36"/>
-      <c r="H91" s="36"/>
-      <c r="I91" s="36"/>
-      <c r="J91" s="36"/>
+      <c r="B91" s="37"/>
+      <c r="C91" s="37"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="37"/>
+      <c r="G91" s="37"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="37"/>
     </row>
     <row r="92" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B92" s="36"/>
-      <c r="C92" s="36"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="36"/>
-      <c r="H92" s="36"/>
-      <c r="I92" s="36"/>
-      <c r="J92" s="36"/>
+      <c r="B92" s="37"/>
+      <c r="C92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="37"/>
     </row>
     <row r="93" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B93" s="36"/>
-      <c r="C93" s="36"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
-      <c r="F93" s="36"/>
-      <c r="G93" s="36"/>
-      <c r="H93" s="36"/>
-      <c r="I93" s="36"/>
-      <c r="J93" s="36"/>
+      <c r="B93" s="37"/>
+      <c r="C93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+      <c r="J93" s="37"/>
     </row>
     <row r="94" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B94" s="36"/>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="36"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="36"/>
-      <c r="I94" s="36"/>
-      <c r="J94" s="36"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="37"/>
     </row>
     <row r="95" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B95" s="36"/>
-      <c r="C95" s="36"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
-      <c r="F95" s="36"/>
-      <c r="G95" s="36"/>
-      <c r="H95" s="36"/>
-      <c r="I95" s="36"/>
-      <c r="J95" s="36"/>
+      <c r="B95" s="37"/>
+      <c r="C95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+      <c r="J95" s="37"/>
     </row>
     <row r="96" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B96" s="36"/>
-      <c r="C96" s="36"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="36"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="36"/>
-      <c r="I96" s="36"/>
-      <c r="J96" s="36"/>
+      <c r="B96" s="37"/>
+      <c r="C96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="37"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="37"/>
     </row>
     <row r="97" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B97" s="36"/>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="36"/>
-      <c r="H97" s="36"/>
-      <c r="I97" s="36"/>
-      <c r="J97" s="36"/>
+      <c r="B97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="37"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="37"/>
     </row>
     <row r="98" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B98" s="36"/>
-      <c r="C98" s="36"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="36"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="36"/>
-      <c r="I98" s="36"/>
-      <c r="J98" s="36"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="37"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="37"/>
     </row>
     <row r="99" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B99" s="36"/>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="36"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="36"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="37"/>
     </row>
     <row r="100" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B100" s="36"/>
-      <c r="C100" s="36"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
-      <c r="F100" s="36"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="36"/>
-      <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
+      <c r="B100" s="37"/>
+      <c r="C100" s="37"/>
+      <c r="D100" s="37"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="37"/>
     </row>
     <row r="101" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B101" s="36"/>
-      <c r="C101" s="36"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
+      <c r="B101" s="37"/>
+      <c r="C101" s="37"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+      <c r="J101" s="37"/>
     </row>
     <row r="102" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B102" s="36"/>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="36"/>
-      <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
+      <c r="B102" s="37"/>
+      <c r="C102" s="37"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+      <c r="J102" s="37"/>
     </row>
     <row r="103" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="36"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="36"/>
-      <c r="I103" s="36"/>
-      <c r="J103" s="36"/>
+      <c r="B103" s="37"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="37"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
+      <c r="J103" s="37"/>
     </row>
     <row r="104" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B104" s="36"/>
-      <c r="C104" s="36"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="36"/>
-      <c r="G104" s="36"/>
-      <c r="H104" s="36"/>
-      <c r="I104" s="36"/>
-      <c r="J104" s="36"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="37"/>
     </row>
     <row r="105" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B105" s="36"/>
-      <c r="C105" s="36"/>
-      <c r="D105" s="36"/>
-      <c r="E105" s="36"/>
-      <c r="F105" s="36"/>
-      <c r="G105" s="36"/>
-      <c r="H105" s="36"/>
-      <c r="I105" s="36"/>
-      <c r="J105" s="36"/>
+      <c r="B105" s="37"/>
+      <c r="C105" s="37"/>
+      <c r="D105" s="37"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="37"/>
+      <c r="H105" s="37"/>
+      <c r="I105" s="37"/>
+      <c r="J105" s="37"/>
     </row>
     <row r="106" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B106" s="36"/>
-      <c r="C106" s="36"/>
-      <c r="D106" s="36"/>
-      <c r="E106" s="36"/>
-      <c r="F106" s="36"/>
-      <c r="G106" s="36"/>
-      <c r="H106" s="36"/>
-      <c r="I106" s="36"/>
-      <c r="J106" s="36"/>
+      <c r="B106" s="37"/>
+      <c r="C106" s="37"/>
+      <c r="D106" s="37"/>
+      <c r="E106" s="37"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+      <c r="J106" s="37"/>
     </row>
     <row r="107" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B107" s="36"/>
-      <c r="C107" s="36"/>
-      <c r="D107" s="36"/>
-      <c r="E107" s="36"/>
-      <c r="F107" s="36"/>
-      <c r="G107" s="36"/>
-      <c r="H107" s="36"/>
-      <c r="I107" s="36"/>
-      <c r="J107" s="36"/>
+      <c r="B107" s="37"/>
+      <c r="C107" s="37"/>
+      <c r="D107" s="37"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="37"/>
     </row>
     <row r="108" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B108" s="36"/>
-      <c r="C108" s="36"/>
-      <c r="D108" s="36"/>
-      <c r="E108" s="36"/>
-      <c r="F108" s="36"/>
-      <c r="G108" s="36"/>
-      <c r="H108" s="36"/>
-      <c r="I108" s="36"/>
-      <c r="J108" s="36"/>
+      <c r="B108" s="37"/>
+      <c r="C108" s="37"/>
+      <c r="D108" s="37"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+      <c r="J108" s="37"/>
     </row>
     <row r="109" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B109" s="36"/>
-      <c r="C109" s="36"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="36"/>
-      <c r="F109" s="36"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="36"/>
-      <c r="J109" s="36"/>
+      <c r="B109" s="37"/>
+      <c r="C109" s="37"/>
+      <c r="D109" s="37"/>
+      <c r="E109" s="37"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+      <c r="J109" s="37"/>
     </row>
     <row r="110" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B110" s="36"/>
-      <c r="C110" s="36"/>
-      <c r="D110" s="36"/>
-      <c r="E110" s="36"/>
-      <c r="F110" s="36"/>
-      <c r="G110" s="36"/>
-      <c r="H110" s="36"/>
-      <c r="I110" s="36"/>
-      <c r="J110" s="36"/>
+      <c r="B110" s="37"/>
+      <c r="C110" s="37"/>
+      <c r="D110" s="37"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="37"/>
+      <c r="H110" s="37"/>
+      <c r="I110" s="37"/>
+      <c r="J110" s="37"/>
     </row>
     <row r="111" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B111" s="36"/>
-      <c r="C111" s="36"/>
-      <c r="D111" s="36"/>
-      <c r="E111" s="36"/>
-      <c r="F111" s="36"/>
-      <c r="G111" s="36"/>
-      <c r="H111" s="36"/>
-      <c r="I111" s="36"/>
-      <c r="J111" s="36"/>
+      <c r="B111" s="37"/>
+      <c r="C111" s="37"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="37"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="37"/>
+      <c r="J111" s="37"/>
     </row>
     <row r="112" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B112" s="36"/>
-      <c r="C112" s="36"/>
-      <c r="D112" s="36"/>
-      <c r="E112" s="36"/>
-      <c r="F112" s="36"/>
-      <c r="G112" s="36"/>
-      <c r="H112" s="36"/>
-      <c r="I112" s="36"/>
-      <c r="J112" s="36"/>
+      <c r="B112" s="37"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="37"/>
+      <c r="G112" s="37"/>
+      <c r="H112" s="37"/>
+      <c r="I112" s="37"/>
+      <c r="J112" s="37"/>
     </row>
     <row r="113" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B113" s="36"/>
-      <c r="C113" s="36"/>
-      <c r="D113" s="36"/>
-      <c r="E113" s="36"/>
-      <c r="F113" s="36"/>
-      <c r="G113" s="36"/>
-      <c r="H113" s="36"/>
-      <c r="I113" s="36"/>
-      <c r="J113" s="36"/>
+      <c r="B113" s="37"/>
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
+      <c r="H113" s="37"/>
+      <c r="I113" s="37"/>
+      <c r="J113" s="37"/>
     </row>
     <row r="114" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B114" s="36"/>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
-      <c r="F114" s="36"/>
-      <c r="G114" s="36"/>
-      <c r="H114" s="36"/>
-      <c r="I114" s="36"/>
-      <c r="J114" s="36"/>
+      <c r="B114" s="37"/>
+      <c r="C114" s="37"/>
+      <c r="D114" s="37"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="37"/>
+      <c r="G114" s="37"/>
+      <c r="H114" s="37"/>
+      <c r="I114" s="37"/>
+      <c r="J114" s="37"/>
     </row>
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B115" s="36"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="36"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="36"/>
-      <c r="I115" s="36"/>
-      <c r="J115" s="36"/>
+      <c r="B115" s="37"/>
+      <c r="C115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="37"/>
+      <c r="G115" s="37"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="37"/>
     </row>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B116" s="36"/>
-      <c r="C116" s="36"/>
-      <c r="D116" s="36"/>
-      <c r="E116" s="36"/>
-      <c r="F116" s="36"/>
-      <c r="G116" s="36"/>
-      <c r="H116" s="36"/>
-      <c r="I116" s="36"/>
-      <c r="J116" s="36"/>
+      <c r="B116" s="37"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="37"/>
     </row>
     <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B118" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C118" s="36"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
-      <c r="F118" s="36"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="36"/>
-      <c r="I118" s="36"/>
-      <c r="J118" s="36"/>
+      <c r="B118" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C118" s="37"/>
+      <c r="D118" s="37"/>
+      <c r="E118" s="37"/>
+      <c r="F118" s="37"/>
+      <c r="G118" s="37"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="37"/>
+      <c r="J118" s="37"/>
     </row>
     <row r="119" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B119" s="36"/>
-      <c r="C119" s="36"/>
-      <c r="D119" s="36"/>
-      <c r="E119" s="36"/>
-      <c r="F119" s="36"/>
-      <c r="G119" s="36"/>
-      <c r="H119" s="36"/>
-      <c r="I119" s="36"/>
-      <c r="J119" s="36"/>
+      <c r="B119" s="37"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="37"/>
+      <c r="E119" s="37"/>
+      <c r="F119" s="37"/>
+      <c r="G119" s="37"/>
+      <c r="H119" s="37"/>
+      <c r="I119" s="37"/>
+      <c r="J119" s="37"/>
     </row>
     <row r="120" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B120" s="36"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="36"/>
-      <c r="E120" s="36"/>
-      <c r="F120" s="36"/>
-      <c r="G120" s="36"/>
-      <c r="H120" s="36"/>
-      <c r="I120" s="36"/>
-      <c r="J120" s="36"/>
+      <c r="B120" s="37"/>
+      <c r="C120" s="37"/>
+      <c r="D120" s="37"/>
+      <c r="E120" s="37"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="37"/>
+      <c r="H120" s="37"/>
+      <c r="I120" s="37"/>
+      <c r="J120" s="37"/>
     </row>
     <row r="121" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B121" s="36"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="36"/>
-      <c r="E121" s="36"/>
-      <c r="F121" s="36"/>
-      <c r="G121" s="36"/>
-      <c r="H121" s="36"/>
-      <c r="I121" s="36"/>
-      <c r="J121" s="36"/>
+      <c r="B121" s="37"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="37"/>
+      <c r="E121" s="37"/>
+      <c r="F121" s="37"/>
+      <c r="G121" s="37"/>
+      <c r="H121" s="37"/>
+      <c r="I121" s="37"/>
+      <c r="J121" s="37"/>
     </row>
     <row r="122" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B122" s="36"/>
-      <c r="C122" s="36"/>
-      <c r="D122" s="36"/>
-      <c r="E122" s="36"/>
-      <c r="F122" s="36"/>
-      <c r="G122" s="36"/>
-      <c r="H122" s="36"/>
-      <c r="I122" s="36"/>
-      <c r="J122" s="36"/>
+      <c r="B122" s="37"/>
+      <c r="C122" s="37"/>
+      <c r="D122" s="37"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="37"/>
+      <c r="G122" s="37"/>
+      <c r="H122" s="37"/>
+      <c r="I122" s="37"/>
+      <c r="J122" s="37"/>
     </row>
     <row r="123" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B123" s="36"/>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
-      <c r="E123" s="36"/>
-      <c r="F123" s="36"/>
-      <c r="G123" s="36"/>
-      <c r="H123" s="36"/>
-      <c r="I123" s="36"/>
-      <c r="J123" s="36"/>
+      <c r="B123" s="37"/>
+      <c r="C123" s="37"/>
+      <c r="D123" s="37"/>
+      <c r="E123" s="37"/>
+      <c r="F123" s="37"/>
+      <c r="G123" s="37"/>
+      <c r="H123" s="37"/>
+      <c r="I123" s="37"/>
+      <c r="J123" s="37"/>
     </row>
     <row r="124" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B124" s="36"/>
-      <c r="C124" s="36"/>
-      <c r="D124" s="36"/>
-      <c r="E124" s="36"/>
-      <c r="F124" s="36"/>
-      <c r="G124" s="36"/>
-      <c r="H124" s="36"/>
-      <c r="I124" s="36"/>
-      <c r="J124" s="36"/>
+      <c r="B124" s="37"/>
+      <c r="C124" s="37"/>
+      <c r="D124" s="37"/>
+      <c r="E124" s="37"/>
+      <c r="F124" s="37"/>
+      <c r="G124" s="37"/>
+      <c r="H124" s="37"/>
+      <c r="I124" s="37"/>
+      <c r="J124" s="37"/>
     </row>
     <row r="125" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B125" s="36"/>
-      <c r="C125" s="36"/>
-      <c r="D125" s="36"/>
-      <c r="E125" s="36"/>
-      <c r="F125" s="36"/>
-      <c r="G125" s="36"/>
-      <c r="H125" s="36"/>
-      <c r="I125" s="36"/>
-      <c r="J125" s="36"/>
+      <c r="B125" s="37"/>
+      <c r="C125" s="37"/>
+      <c r="D125" s="37"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="37"/>
+      <c r="G125" s="37"/>
+      <c r="H125" s="37"/>
+      <c r="I125" s="37"/>
+      <c r="J125" s="37"/>
     </row>
     <row r="126" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B126" s="36"/>
-      <c r="C126" s="36"/>
-      <c r="D126" s="36"/>
-      <c r="E126" s="36"/>
-      <c r="F126" s="36"/>
-      <c r="G126" s="36"/>
-      <c r="H126" s="36"/>
-      <c r="I126" s="36"/>
-      <c r="J126" s="36"/>
+      <c r="B126" s="37"/>
+      <c r="C126" s="37"/>
+      <c r="D126" s="37"/>
+      <c r="E126" s="37"/>
+      <c r="F126" s="37"/>
+      <c r="G126" s="37"/>
+      <c r="H126" s="37"/>
+      <c r="I126" s="37"/>
+      <c r="J126" s="37"/>
     </row>
     <row r="127" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B127" s="36"/>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
-      <c r="E127" s="36"/>
-      <c r="F127" s="36"/>
-      <c r="G127" s="36"/>
-      <c r="H127" s="36"/>
-      <c r="I127" s="36"/>
-      <c r="J127" s="36"/>
+      <c r="B127" s="37"/>
+      <c r="C127" s="37"/>
+      <c r="D127" s="37"/>
+      <c r="E127" s="37"/>
+      <c r="F127" s="37"/>
+      <c r="G127" s="37"/>
+      <c r="H127" s="37"/>
+      <c r="I127" s="37"/>
+      <c r="J127" s="37"/>
     </row>
     <row r="128" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B128" s="36"/>
-      <c r="C128" s="36"/>
-      <c r="D128" s="36"/>
-      <c r="E128" s="36"/>
-      <c r="F128" s="36"/>
-      <c r="G128" s="36"/>
-      <c r="H128" s="36"/>
-      <c r="I128" s="36"/>
-      <c r="J128" s="36"/>
+      <c r="B128" s="37"/>
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
+      <c r="E128" s="37"/>
+      <c r="F128" s="37"/>
+      <c r="G128" s="37"/>
+      <c r="H128" s="37"/>
+      <c r="I128" s="37"/>
+      <c r="J128" s="37"/>
     </row>
     <row r="129" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B129" s="36"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="36"/>
-      <c r="E129" s="36"/>
-      <c r="F129" s="36"/>
-      <c r="G129" s="36"/>
-      <c r="H129" s="36"/>
-      <c r="I129" s="36"/>
-      <c r="J129" s="36"/>
+      <c r="B129" s="37"/>
+      <c r="C129" s="37"/>
+      <c r="D129" s="37"/>
+      <c r="E129" s="37"/>
+      <c r="F129" s="37"/>
+      <c r="G129" s="37"/>
+      <c r="H129" s="37"/>
+      <c r="I129" s="37"/>
+      <c r="J129" s="37"/>
     </row>
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B130" s="36"/>
-      <c r="C130" s="36"/>
-      <c r="D130" s="36"/>
-      <c r="E130" s="36"/>
-      <c r="F130" s="36"/>
-      <c r="G130" s="36"/>
-      <c r="H130" s="36"/>
-      <c r="I130" s="36"/>
-      <c r="J130" s="36"/>
+      <c r="B130" s="37"/>
+      <c r="C130" s="37"/>
+      <c r="D130" s="37"/>
+      <c r="E130" s="37"/>
+      <c r="F130" s="37"/>
+      <c r="G130" s="37"/>
+      <c r="H130" s="37"/>
+      <c r="I130" s="37"/>
+      <c r="J130" s="37"/>
     </row>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B131" s="36"/>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
-      <c r="F131" s="36"/>
-      <c r="G131" s="36"/>
-      <c r="H131" s="36"/>
-      <c r="I131" s="36"/>
-      <c r="J131" s="36"/>
+      <c r="B131" s="37"/>
+      <c r="C131" s="37"/>
+      <c r="D131" s="37"/>
+      <c r="E131" s="37"/>
+      <c r="F131" s="37"/>
+      <c r="G131" s="37"/>
+      <c r="H131" s="37"/>
+      <c r="I131" s="37"/>
+      <c r="J131" s="37"/>
     </row>
     <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B133" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C133" s="36"/>
-      <c r="D133" s="36"/>
-      <c r="E133" s="36"/>
-      <c r="F133" s="36"/>
-      <c r="G133" s="36"/>
-      <c r="H133" s="36"/>
-      <c r="I133" s="36"/>
-      <c r="J133" s="36"/>
+      <c r="B133" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C133" s="37"/>
+      <c r="D133" s="37"/>
+      <c r="E133" s="37"/>
+      <c r="F133" s="37"/>
+      <c r="G133" s="37"/>
+      <c r="H133" s="37"/>
+      <c r="I133" s="37"/>
+      <c r="J133" s="37"/>
     </row>
     <row r="134" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B134" s="36"/>
-      <c r="C134" s="36"/>
-      <c r="D134" s="36"/>
-      <c r="E134" s="36"/>
-      <c r="F134" s="36"/>
-      <c r="G134" s="36"/>
-      <c r="H134" s="36"/>
-      <c r="I134" s="36"/>
-      <c r="J134" s="36"/>
+      <c r="B134" s="37"/>
+      <c r="C134" s="37"/>
+      <c r="D134" s="37"/>
+      <c r="E134" s="37"/>
+      <c r="F134" s="37"/>
+      <c r="G134" s="37"/>
+      <c r="H134" s="37"/>
+      <c r="I134" s="37"/>
+      <c r="J134" s="37"/>
     </row>
     <row r="135" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B135" s="36"/>
-      <c r="C135" s="36"/>
-      <c r="D135" s="36"/>
-      <c r="E135" s="36"/>
-      <c r="F135" s="36"/>
-      <c r="G135" s="36"/>
-      <c r="H135" s="36"/>
-      <c r="I135" s="36"/>
-      <c r="J135" s="36"/>
+      <c r="B135" s="37"/>
+      <c r="C135" s="37"/>
+      <c r="D135" s="37"/>
+      <c r="E135" s="37"/>
+      <c r="F135" s="37"/>
+      <c r="G135" s="37"/>
+      <c r="H135" s="37"/>
+      <c r="I135" s="37"/>
+      <c r="J135" s="37"/>
     </row>
     <row r="136" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B136" s="36"/>
-      <c r="C136" s="36"/>
-      <c r="D136" s="36"/>
-      <c r="E136" s="36"/>
-      <c r="F136" s="36"/>
-      <c r="G136" s="36"/>
-      <c r="H136" s="36"/>
-      <c r="I136" s="36"/>
-      <c r="J136" s="36"/>
+      <c r="B136" s="37"/>
+      <c r="C136" s="37"/>
+      <c r="D136" s="37"/>
+      <c r="E136" s="37"/>
+      <c r="F136" s="37"/>
+      <c r="G136" s="37"/>
+      <c r="H136" s="37"/>
+      <c r="I136" s="37"/>
+      <c r="J136" s="37"/>
     </row>
     <row r="137" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B137" s="36"/>
-      <c r="C137" s="36"/>
-      <c r="D137" s="36"/>
-      <c r="E137" s="36"/>
-      <c r="F137" s="36"/>
-      <c r="G137" s="36"/>
-      <c r="H137" s="36"/>
-      <c r="I137" s="36"/>
-      <c r="J137" s="36"/>
+      <c r="B137" s="37"/>
+      <c r="C137" s="37"/>
+      <c r="D137" s="37"/>
+      <c r="E137" s="37"/>
+      <c r="F137" s="37"/>
+      <c r="G137" s="37"/>
+      <c r="H137" s="37"/>
+      <c r="I137" s="37"/>
+      <c r="J137" s="37"/>
     </row>
     <row r="138" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B138" s="36"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="36"/>
-      <c r="E138" s="36"/>
-      <c r="F138" s="36"/>
-      <c r="G138" s="36"/>
-      <c r="H138" s="36"/>
-      <c r="I138" s="36"/>
-      <c r="J138" s="36"/>
+      <c r="B138" s="37"/>
+      <c r="C138" s="37"/>
+      <c r="D138" s="37"/>
+      <c r="E138" s="37"/>
+      <c r="F138" s="37"/>
+      <c r="G138" s="37"/>
+      <c r="H138" s="37"/>
+      <c r="I138" s="37"/>
+      <c r="J138" s="37"/>
     </row>
     <row r="139" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B139" s="36"/>
-      <c r="C139" s="36"/>
-      <c r="D139" s="36"/>
-      <c r="E139" s="36"/>
-      <c r="F139" s="36"/>
-      <c r="G139" s="36"/>
-      <c r="H139" s="36"/>
-      <c r="I139" s="36"/>
-      <c r="J139" s="36"/>
+      <c r="B139" s="37"/>
+      <c r="C139" s="37"/>
+      <c r="D139" s="37"/>
+      <c r="E139" s="37"/>
+      <c r="F139" s="37"/>
+      <c r="G139" s="37"/>
+      <c r="H139" s="37"/>
+      <c r="I139" s="37"/>
+      <c r="J139" s="37"/>
     </row>
     <row r="140" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B140" s="36"/>
-      <c r="C140" s="36"/>
-      <c r="D140" s="36"/>
-      <c r="E140" s="36"/>
-      <c r="F140" s="36"/>
-      <c r="G140" s="36"/>
-      <c r="H140" s="36"/>
-      <c r="I140" s="36"/>
-      <c r="J140" s="36"/>
+      <c r="B140" s="37"/>
+      <c r="C140" s="37"/>
+      <c r="D140" s="37"/>
+      <c r="E140" s="37"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="37"/>
+      <c r="H140" s="37"/>
+      <c r="I140" s="37"/>
+      <c r="J140" s="37"/>
     </row>
     <row r="141" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B141" s="36"/>
-      <c r="C141" s="36"/>
-      <c r="D141" s="36"/>
-      <c r="E141" s="36"/>
-      <c r="F141" s="36"/>
-      <c r="G141" s="36"/>
-      <c r="H141" s="36"/>
-      <c r="I141" s="36"/>
-      <c r="J141" s="36"/>
+      <c r="B141" s="37"/>
+      <c r="C141" s="37"/>
+      <c r="D141" s="37"/>
+      <c r="E141" s="37"/>
+      <c r="F141" s="37"/>
+      <c r="G141" s="37"/>
+      <c r="H141" s="37"/>
+      <c r="I141" s="37"/>
+      <c r="J141" s="37"/>
     </row>
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B143" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C143" s="38"/>
-      <c r="D143" s="38"/>
-      <c r="E143" s="38"/>
-      <c r="F143" s="38"/>
-      <c r="G143" s="38"/>
-      <c r="H143" s="38"/>
-      <c r="I143" s="38"/>
-      <c r="J143" s="38"/>
+      <c r="B143" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C143" s="39"/>
+      <c r="D143" s="39"/>
+      <c r="E143" s="39"/>
+      <c r="F143" s="39"/>
+      <c r="G143" s="39"/>
+      <c r="H143" s="39"/>
+      <c r="I143" s="39"/>
+      <c r="J143" s="39"/>
     </row>
     <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B144" s="38"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="38"/>
-      <c r="E144" s="38"/>
-      <c r="F144" s="38"/>
-      <c r="G144" s="38"/>
-      <c r="H144" s="38"/>
-      <c r="I144" s="38"/>
-      <c r="J144" s="38"/>
+      <c r="B144" s="39"/>
+      <c r="C144" s="39"/>
+      <c r="D144" s="39"/>
+      <c r="E144" s="39"/>
+      <c r="F144" s="39"/>
+      <c r="G144" s="39"/>
+      <c r="H144" s="39"/>
+      <c r="I144" s="39"/>
+      <c r="J144" s="39"/>
     </row>
     <row r="145" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B145" s="38"/>
-      <c r="C145" s="38"/>
-      <c r="D145" s="38"/>
-      <c r="E145" s="38"/>
-      <c r="F145" s="38"/>
-      <c r="G145" s="38"/>
-      <c r="H145" s="38"/>
-      <c r="I145" s="38"/>
-      <c r="J145" s="38"/>
+      <c r="B145" s="39"/>
+      <c r="C145" s="39"/>
+      <c r="D145" s="39"/>
+      <c r="E145" s="39"/>
+      <c r="F145" s="39"/>
+      <c r="G145" s="39"/>
+      <c r="H145" s="39"/>
+      <c r="I145" s="39"/>
+      <c r="J145" s="39"/>
     </row>
     <row r="146" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B146" s="38"/>
-      <c r="C146" s="38"/>
-      <c r="D146" s="38"/>
-      <c r="E146" s="38"/>
-      <c r="F146" s="38"/>
-      <c r="G146" s="38"/>
-      <c r="H146" s="38"/>
-      <c r="I146" s="38"/>
-      <c r="J146" s="38"/>
+      <c r="B146" s="39"/>
+      <c r="C146" s="39"/>
+      <c r="D146" s="39"/>
+      <c r="E146" s="39"/>
+      <c r="F146" s="39"/>
+      <c r="G146" s="39"/>
+      <c r="H146" s="39"/>
+      <c r="I146" s="39"/>
+      <c r="J146" s="39"/>
     </row>
     <row r="147" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B147" s="38"/>
-      <c r="C147" s="38"/>
-      <c r="D147" s="38"/>
-      <c r="E147" s="38"/>
-      <c r="F147" s="38"/>
-      <c r="G147" s="38"/>
-      <c r="H147" s="38"/>
-      <c r="I147" s="38"/>
-      <c r="J147" s="38"/>
+      <c r="B147" s="39"/>
+      <c r="C147" s="39"/>
+      <c r="D147" s="39"/>
+      <c r="E147" s="39"/>
+      <c r="F147" s="39"/>
+      <c r="G147" s="39"/>
+      <c r="H147" s="39"/>
+      <c r="I147" s="39"/>
+      <c r="J147" s="39"/>
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="17" t="s">
@@ -5208,9 +5219,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D994"/>
+  <dimension ref="A1:D995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5359,7 +5370,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="36" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6341,6 +6365,7 @@
     <row r="992" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -6376,7 +6401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>47</v>
       </c>
@@ -6396,13 +6421,13 @@
         <v>52</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -6455,7 +6480,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6463,19 +6488,19 @@
         <v>47</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="F2" s="23" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6982,24 +7007,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="C2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="D2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -7044,10 +7069,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change default view of template to Concepts Sheet
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76FE9C2-B719-4322-A919-24F5CE758CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6D2A4D-C58C-4C65-9AE5-B39DDBBA9B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="28260" windowHeight="16380" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="28260" windowHeight="16380" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -2352,7 +2352,7 @@
   </sheetPr>
   <dimension ref="A11:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -6379,7 +6379,7 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>